<commit_message>
03.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Raju Ahamed" sheetId="1" r:id="rId2"/>
     <sheet name="A.M Tipu" sheetId="2" r:id="rId3"/>
     <sheet name="Mithu Jaman" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="26">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -81,17 +83,32 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 30.06.19</t>
+    <t>Date: 02.07.19</t>
   </si>
   <si>
-    <t>Date: 01.07.19</t>
+    <t>Dealer Conveyance April'2019</t>
+  </si>
+  <si>
+    <t>Dealer Conveyance May'2019</t>
+  </si>
+  <si>
+    <t>Dealer On hand Stock Adj.(B12i,D10,D22,D38i,D54j)</t>
+  </si>
+  <si>
+    <t>Dealer On hand Stock Adj.(E90,V48,V92,V94)</t>
+  </si>
+  <si>
+    <t>Total=</t>
+  </si>
+  <si>
+    <t>Date: 03.07.19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +200,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -198,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -247,11 +272,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -287,6 +374,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -358,6 +457,36 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,6 +1379,280 @@
         <a:xfrm>
           <a:off x="47625" y="5353050"/>
           <a:ext cx="1190625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="5353050"/>
+          <a:ext cx="1190625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6953250" y="5334000"/>
+          <a:ext cx="1466850" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>11113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="12744450"/>
+          <a:ext cx="1228725" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6962775" y="12725400"/>
+          <a:ext cx="1457325" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>11113</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525" y="10791825"/>
+          <a:ext cx="1209675" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6972300" y="10772775"/>
+          <a:ext cx="1838325" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1541,7 +1944,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:F8"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1552,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1614,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1632,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="27">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1651,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="27">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1670,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="27">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1689,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="27">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1708,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1725,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1739,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1789,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1850,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1929,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1991,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2009,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="27">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2028,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="27">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2047,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="27">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2066,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="27">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2085,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2102,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2116,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2166,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2227,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2308,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2327,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="A4" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2393,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2411,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>59</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="27">
+        <v>35</v>
+      </c>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>59000</v>
+        <v>35000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2430,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>161</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="27">
+        <v>87</v>
+      </c>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>80500</v>
+        <v>43500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2449,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>285</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="27">
+        <v>262</v>
+      </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>28500</v>
+        <v>26200</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2468,13 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>100</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="27">
+        <v>116</v>
+      </c>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>5800</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2487,11 +2890,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="27">
+        <v>25</v>
+      </c>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2504,11 +2909,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="27">
+        <v>100</v>
+      </c>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2518,14 +2925,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>173000</v>
+        <v>112000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2568,58 +2975,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2629,9 +3036,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2718,60 +3125,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="A31" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2782,10 +3189,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2800,13 +3207,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>59</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="27">
+        <v>35</v>
+      </c>
+      <c r="F33" s="27"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>59000</v>
+        <v>35000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2819,13 +3226,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>161</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="27">
+        <v>87</v>
+      </c>
+      <c r="F34" s="27"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>80500</v>
+        <v>43500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2838,13 +3245,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>285</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="27">
+        <v>262</v>
+      </c>
+      <c r="F35" s="27"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>28500</v>
+        <v>26200</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2857,13 +3264,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
-        <v>100</v>
-      </c>
-      <c r="F36" s="23"/>
+      <c r="E36" s="27">
+        <v>116</v>
+      </c>
+      <c r="F36" s="27"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>5800</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2876,11 +3283,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="35">
+        <v>25</v>
+      </c>
+      <c r="F37" s="35"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2893,11 +3302,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="35">
+        <v>100</v>
+      </c>
+      <c r="F38" s="35"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2907,14 +3318,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>173000</v>
+        <v>112000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2957,58 +3368,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3018,9 +3429,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3116,63 +3527,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3182,10 +3593,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3200,10 +3611,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="27">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3219,10 +3630,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="27">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3238,10 +3649,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="27">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3257,10 +3668,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="27">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3276,10 +3687,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="27">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3295,8 +3706,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3309,10 +3720,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3359,76 +3770,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3503,60 +3914,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3565,10 +3976,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3583,10 +3994,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="35">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3602,10 +4013,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="35">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3621,10 +4032,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="35">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3640,10 +4051,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="35">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3659,10 +4070,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="35">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3678,8 +4089,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3692,10 +4103,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="37"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -3742,76 +4153,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="36"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3910,63 +4321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3976,10 +4387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3994,10 +4405,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="27">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4013,10 +4424,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="27">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4032,10 +4443,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="27">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4051,8 +4462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4068,8 +4479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4085,8 +4496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4099,10 +4510,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4149,72 +4560,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4289,60 +4700,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4351,10 +4762,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4369,10 +4780,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="27">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4388,10 +4799,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="27">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4407,10 +4818,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="27">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4426,8 +4837,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4443,8 +4854,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4460,8 +4871,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4474,10 +4885,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4524,72 +4935,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4663,4 +5074,1178 @@
   <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:J47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="31.5">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+    </row>
+    <row r="4" spans="1:10" ht="18.75">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" ht="23.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="23.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="23.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="23.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="23.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="23.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="23.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" ht="31.5">
+      <c r="A28" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+    </row>
+    <row r="29" spans="1:10" ht="18">
+      <c r="A29" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75">
+      <c r="A30" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" spans="1:10" ht="18.75">
+      <c r="A31" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+    </row>
+    <row r="32" spans="1:10" ht="20.25">
+      <c r="A32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="38"/>
+      <c r="G32" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="23.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="19">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="27">
+        <v>30</v>
+      </c>
+      <c r="F33" s="27"/>
+      <c r="G33" s="19">
+        <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
+        <v>30000</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="23.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="19">
+        <v>500</v>
+      </c>
+      <c r="E34" s="27">
+        <v>35</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="G34" s="19">
+        <f t="shared" si="0"/>
+        <v>17500</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="23.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="19">
+        <v>100</v>
+      </c>
+      <c r="E35" s="27">
+        <v>425</v>
+      </c>
+      <c r="F35" s="27"/>
+      <c r="G35" s="19">
+        <f t="shared" si="0"/>
+        <v>42500</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="23.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="19">
+        <v>50</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="20.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="19">
+        <v>20</v>
+      </c>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="19">
+        <f>SUM(D37*E37)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="20.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="19">
+        <v>10</v>
+      </c>
+      <c r="E38" s="35">
+        <v>100</v>
+      </c>
+      <c r="F38" s="35"/>
+      <c r="G38" s="19">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10" ht="20.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="37"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20">
+        <f>SUM(G33:G38)</f>
+        <v>91000</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75">
+      <c r="A43" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="25"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="31.5">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" ht="18">
+      <c r="A2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="44">
+        <v>1</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="46">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="44"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="46"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="44">
+        <v>2</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="46">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="44"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="46"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="44">
+        <v>3</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="46">
+        <v>10538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="44"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="46"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="44">
+        <v>4</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="46">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="44"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="46"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="46">
+        <f>SUM(G5:G12)</f>
+        <v>15268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="45"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75">
+      <c r="A23" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" spans="1:10" ht="18.75">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+    </row>
+    <row r="25" spans="1:10" ht="20.25">
+      <c r="A25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="38"/>
+      <c r="G25" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="23.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="19">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="19">
+        <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="23.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="19">
+        <v>500</v>
+      </c>
+      <c r="E27" s="27">
+        <v>30</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="19">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" ht="23.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="19">
+        <v>100</v>
+      </c>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" ht="23.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="19">
+        <v>50</v>
+      </c>
+      <c r="E29" s="27">
+        <v>5</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="19">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" ht="20.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="19">
+        <v>20</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="19">
+        <f>SUM(D30*E30)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" ht="20.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="19">
+        <v>10</v>
+      </c>
+      <c r="E31" s="35">
+        <v>2</v>
+      </c>
+      <c r="F31" s="35"/>
+      <c r="G31" s="19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="20.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="37"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20">
+        <f>SUM(G26:G31)</f>
+        <v>15270</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="15.75">
+      <c r="A36" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75">
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="G13:G14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="71" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
04.07.19 Today Sales Detals
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 03.07.19</t>
+    <t>Date: 04.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,11 +388,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -403,36 +430,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -440,6 +437,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,20 +451,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -486,6 +477,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>50</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>16</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>151</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>58</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>50</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>116</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>151</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>58</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,6 +2662,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2674,32 +2700,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
-        <v>35</v>
-      </c>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25">
+        <v>38</v>
+      </c>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>35000</v>
+        <v>38000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
-        <v>87</v>
-      </c>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25">
+        <v>121</v>
+      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>43500</v>
+        <v>60500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
-        <v>262</v>
-      </c>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25">
+        <v>178</v>
+      </c>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>26200</v>
+        <v>17800</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,13 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
-        <v>116</v>
-      </c>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25">
+        <v>14</v>
+      </c>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>5800</v>
+        <v>700</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,13 +2890,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
-        <v>25</v>
-      </c>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2909,13 +2907,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27">
-        <v>100</v>
-      </c>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2925,14 +2921,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>112000</v>
+        <v>117000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2975,58 +2971,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3036,9 +3032,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3125,60 +3121,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3189,10 +3185,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -3207,13 +3203,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
-        <v>35</v>
-      </c>
-      <c r="F33" s="27"/>
+      <c r="E33" s="25">
+        <v>38</v>
+      </c>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>35000</v>
+        <v>38000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3226,13 +3222,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
-        <v>87</v>
-      </c>
-      <c r="F34" s="27"/>
+      <c r="E34" s="25">
+        <v>121</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>43500</v>
+        <v>60500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3245,13 +3241,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
-        <v>262</v>
-      </c>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25">
+        <v>178</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>26200</v>
+        <v>17800</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3264,13 +3260,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="27">
-        <v>116</v>
-      </c>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25">
+        <v>14</v>
+      </c>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>5800</v>
+        <v>700</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3283,13 +3279,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="35">
-        <v>25</v>
-      </c>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3302,13 +3296,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
-        <v>100</v>
-      </c>
-      <c r="F38" s="35"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3318,14 +3310,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>112000</v>
+        <v>117000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3368,58 +3360,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3429,9 +3421,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3459,6 +3451,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3475,28 +3489,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3527,63 +3519,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3593,10 +3585,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3611,10 +3603,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>68</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3630,10 +3622,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>135</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3649,10 +3641,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>53</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3668,10 +3660,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>2</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3687,10 +3679,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3706,8 +3698,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3720,10 +3712,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3770,60 +3762,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="39" t="s">
@@ -3835,11 +3827,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3914,60 +3906,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3976,10 +3968,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3994,10 +3986,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="35">
+      <c r="E32" s="38">
         <v>68</v>
       </c>
-      <c r="F32" s="35"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4013,10 +4005,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="38">
         <v>135</v>
       </c>
-      <c r="F33" s="35"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4032,10 +4024,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E34" s="38">
         <v>53</v>
       </c>
-      <c r="F34" s="35"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4051,10 +4043,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="38">
         <v>2</v>
       </c>
-      <c r="F35" s="35"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4070,10 +4062,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="38">
         <v>5</v>
       </c>
-      <c r="F36" s="35"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4089,8 +4081,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4153,60 +4145,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40" t="s">
@@ -4218,11 +4210,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4250,6 +4242,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4266,30 +4282,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4321,63 +4313,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4387,10 +4379,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4405,10 +4397,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>44</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4424,10 +4416,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>118</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4443,10 +4435,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>510</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4462,8 +4454,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4479,8 +4471,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4496,8 +4488,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4510,10 +4502,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4560,72 +4552,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4700,60 +4692,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4762,10 +4754,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4780,10 +4772,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4799,10 +4791,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>118</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4818,10 +4810,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>510</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4837,8 +4829,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4854,8 +4846,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4871,8 +4863,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4885,10 +4877,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4935,58 +4927,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40"/>
@@ -4996,11 +4988,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5028,16 +5020,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5050,24 +5050,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5092,64 +5084,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5160,8 +5152,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5172,8 +5164,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5184,8 +5176,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5196,8 +5188,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5208,8 +5200,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5220,8 +5212,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5231,8 +5223,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5276,52 +5268,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5331,9 +5323,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5420,60 +5412,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5484,10 +5476,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5502,10 +5494,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>30</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5521,10 +5513,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>35</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5540,10 +5532,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>425</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5559,8 +5551,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5576,8 +5568,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5593,10 +5585,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
+      <c r="E38" s="38">
         <v>100</v>
       </c>
-      <c r="F38" s="35"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5609,10 +5601,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5659,58 +5651,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5720,12 +5712,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5738,32 +5756,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5789,177 +5781,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="44">
+      <c r="A5" s="52">
         <v>1</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="46">
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="51">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="44"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="46"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="44">
+      <c r="A7" s="52">
         <v>2</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="46">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="51">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="44"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="44">
+      <c r="A9" s="52">
         <v>3</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="46">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="51">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="44"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="46"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="44">
+      <c r="A11" s="52">
         <v>4</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="46">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="51">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="44"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="46"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="46">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="51">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="45"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="51"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5970,10 +5962,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -5988,8 +5980,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6005,10 +5997,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="25">
         <v>30</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6024,8 +6016,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6041,10 +6033,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <v>5</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6060,8 +6052,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6077,10 +6069,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="38">
         <v>2</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6093,10 +6085,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6143,58 +6135,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6204,24 +6196,13 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6238,11 +6219,22 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:F14"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
07.07.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 04.07.19</t>
+    <t>Date: 07.07.19</t>
   </si>
 </sst>
 </file>
@@ -457,6 +457,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -482,9 +485,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2712,7 +2712,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+      <selection activeCell="K47" sqref="A1:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2815,12 +2815,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="25">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>38000</v>
+        <v>44000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2834,12 +2834,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="25">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>60500</v>
+        <v>52000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2853,12 +2853,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="25">
-        <v>178</v>
+        <v>326</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>17800</v>
+        <v>32600</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2872,12 +2872,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="25">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,11 +2890,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25">
+        <v>69</v>
+      </c>
       <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2907,11 +2909,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="25">
+        <v>112</v>
+      </c>
       <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2928,7 +2932,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>117000</v>
+        <v>132000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -3204,12 +3208,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="25">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>38000</v>
+        <v>44000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3223,12 +3227,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="25">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>60500</v>
+        <v>52000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3242,12 +3246,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="25">
-        <v>178</v>
+        <v>326</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>17800</v>
+        <v>32600</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3261,12 +3265,12 @@
         <v>50</v>
       </c>
       <c r="E36" s="25">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3279,11 +3283,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="38">
+        <v>69</v>
+      </c>
       <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3296,11 +3302,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="38">
+        <v>112</v>
+      </c>
       <c r="F38" s="38"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3317,7 +3325,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>117000</v>
+        <v>132000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -5809,123 +5817,123 @@
       <c r="J2" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="52">
+      <c r="A5" s="53">
         <v>1</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="51">
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="52">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="52"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="51"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="52">
+      <c r="A7" s="53">
         <v>2</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="51">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="52">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="52"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="51"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="52"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="52">
+      <c r="A9" s="53">
         <v>3</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="51">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="52">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="52"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="51"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="52">
+      <c r="A11" s="53">
         <v>4</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="51">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="52"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="51">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="52">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="51"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="52"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
       <c r="A23" s="31" t="s">
@@ -6202,7 +6210,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6218,10 +6225,6 @@
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6234,7 +6237,12 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
09.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 08.07.19</t>
+    <t>Date: 09.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,11 +388,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -403,36 +430,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -440,6 +437,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,20 +451,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -483,6 +477,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>50</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>16</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>151</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>58</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>50</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>116</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>151</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>58</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,6 +2662,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2674,32 +2700,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
-        <v>37</v>
-      </c>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25">
+        <v>49</v>
+      </c>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>37000</v>
+        <v>49000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
-        <v>76</v>
-      </c>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25">
+        <v>152</v>
+      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>38000</v>
+        <v>76000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
-        <v>185</v>
-      </c>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25">
+        <v>70</v>
+      </c>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>18500</v>
+        <v>7000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,13 +2871,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
-        <v>8</v>
-      </c>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,13 +2888,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
-        <v>20</v>
-      </c>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2909,13 +2905,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27">
-        <v>70</v>
-      </c>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2925,14 +2919,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>95000</v>
+        <v>132000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2975,58 +2969,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3036,9 +3030,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3125,60 +3119,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3189,10 +3183,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -3207,13 +3201,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
-        <v>37</v>
-      </c>
-      <c r="F33" s="27"/>
+      <c r="E33" s="25">
+        <v>49</v>
+      </c>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>37000</v>
+        <v>49000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3226,13 +3220,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
-        <v>76</v>
-      </c>
-      <c r="F34" s="27"/>
+      <c r="E34" s="25">
+        <v>152</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>38000</v>
+        <v>76000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3245,13 +3239,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
-        <v>185</v>
-      </c>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25">
+        <v>70</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>18500</v>
+        <v>7000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3264,13 +3258,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="27">
-        <v>8</v>
-      </c>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3283,13 +3275,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="35">
-        <v>20</v>
-      </c>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3302,13 +3292,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
-        <v>70</v>
-      </c>
-      <c r="F38" s="35"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3318,14 +3306,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>95000</v>
+        <v>132000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3368,58 +3356,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3429,9 +3417,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3459,6 +3447,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3475,28 +3485,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3527,63 +3515,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3593,10 +3581,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3611,10 +3599,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>68</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3630,10 +3618,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>135</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3649,10 +3637,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>53</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3668,10 +3656,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>2</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3687,10 +3675,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3706,8 +3694,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3720,10 +3708,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3770,60 +3758,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="39" t="s">
@@ -3835,11 +3823,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3914,60 +3902,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3976,10 +3964,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3994,10 +3982,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="35">
+      <c r="E32" s="38">
         <v>68</v>
       </c>
-      <c r="F32" s="35"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4013,10 +4001,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="38">
         <v>135</v>
       </c>
-      <c r="F33" s="35"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4032,10 +4020,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E34" s="38">
         <v>53</v>
       </c>
-      <c r="F34" s="35"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4051,10 +4039,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="38">
         <v>2</v>
       </c>
-      <c r="F35" s="35"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4070,10 +4058,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="38">
         <v>5</v>
       </c>
-      <c r="F36" s="35"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4089,8 +4077,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4153,60 +4141,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40" t="s">
@@ -4218,11 +4206,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4250,6 +4238,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4266,30 +4278,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4321,63 +4309,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4387,10 +4375,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4405,10 +4393,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>44</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4424,10 +4412,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>118</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4443,10 +4431,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>510</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4462,8 +4450,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4479,8 +4467,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4496,8 +4484,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4510,10 +4498,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4560,72 +4548,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4700,60 +4688,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4762,10 +4750,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4780,10 +4768,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4799,10 +4787,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>118</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4818,10 +4806,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>510</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4837,8 +4825,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4854,8 +4842,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4871,8 +4859,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4885,10 +4873,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4935,58 +4923,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40"/>
@@ -4996,11 +4984,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5028,16 +5016,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5050,24 +5046,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5092,64 +5080,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5160,8 +5148,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5172,8 +5160,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5184,8 +5172,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5196,8 +5184,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5208,8 +5196,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5220,8 +5208,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5231,8 +5219,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5276,52 +5264,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5331,9 +5319,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5420,60 +5408,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5484,10 +5472,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5502,10 +5490,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>30</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5521,10 +5509,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>35</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5540,10 +5528,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>425</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5559,8 +5547,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5576,8 +5564,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5593,10 +5581,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
+      <c r="E38" s="38">
         <v>100</v>
       </c>
-      <c r="F38" s="35"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5609,10 +5597,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5659,58 +5647,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5720,12 +5708,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5738,32 +5752,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5789,128 +5777,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="44">
+      <c r="A5" s="52">
         <v>1</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="46">
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="51">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="44">
+      <c r="A7" s="52">
         <v>2</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="51">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="44">
+      <c r="A9" s="52">
         <v>3</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="51">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="44">
+      <c r="A11" s="52">
         <v>4</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="46">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="51">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="44"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="46"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="53" t="s">
@@ -5921,7 +5909,7 @@
       <c r="D13" s="53"/>
       <c r="E13" s="53"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="46">
+      <c r="G13" s="51">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
@@ -5933,33 +5921,33 @@
       <c r="D14" s="53"/>
       <c r="E14" s="53"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="46"/>
+      <c r="G14" s="51"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5970,10 +5958,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -5988,8 +5976,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6005,10 +5993,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="25">
         <v>30</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6024,8 +6012,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6041,10 +6029,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <v>5</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6060,8 +6048,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6077,10 +6065,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="38">
         <v>2</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6093,10 +6081,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6143,58 +6131,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6204,12 +6192,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="E31:F31"/>
@@ -6226,23 +6231,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
10.07.19 Today Sales details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 09.07.19</t>
+    <t>Date: 10.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,38 +388,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -430,6 +403,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -437,9 +440,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,14 +451,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -477,15 +486,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>50</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>16</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>151</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>58</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="27">
         <v>50</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>116</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>151</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="27">
         <v>58</v>
       </c>
-      <c r="F35" s="25"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,14 +2662,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2682,24 +2692,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2711,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
-        <v>49</v>
-      </c>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27">
+        <v>22</v>
+      </c>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>49000</v>
+        <v>22000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
-        <v>152</v>
-      </c>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27">
+        <v>85</v>
+      </c>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>76000</v>
+        <v>42500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
-        <v>70</v>
-      </c>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27">
+        <v>82</v>
+      </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>8200</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,11 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27">
+        <v>200</v>
+      </c>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2888,11 +2890,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27">
+        <v>15</v>
+      </c>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2905,11 +2909,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27">
+        <v>200</v>
+      </c>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2919,14 +2925,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>132000</v>
+        <v>85000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2969,58 +2975,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3030,9 +3036,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3119,60 +3125,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3183,10 +3189,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -3201,13 +3207,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="25">
-        <v>49</v>
-      </c>
-      <c r="F33" s="25"/>
+      <c r="E33" s="27">
+        <v>22</v>
+      </c>
+      <c r="F33" s="27"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>49000</v>
+        <v>22000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3220,13 +3226,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="25">
-        <v>152</v>
-      </c>
-      <c r="F34" s="25"/>
+      <c r="E34" s="27">
+        <v>85</v>
+      </c>
+      <c r="F34" s="27"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>76000</v>
+        <v>42500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3239,13 +3245,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
-        <v>70</v>
-      </c>
-      <c r="F35" s="25"/>
+      <c r="E35" s="27">
+        <v>82</v>
+      </c>
+      <c r="F35" s="27"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>7000</v>
+        <v>8200</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3258,11 +3264,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27">
+        <v>200</v>
+      </c>
+      <c r="F36" s="27"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3275,11 +3283,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="35">
+        <v>15</v>
+      </c>
+      <c r="F37" s="35"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3292,11 +3302,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
+      <c r="E38" s="35">
+        <v>200</v>
+      </c>
+      <c r="F38" s="35"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3306,14 +3318,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>132000</v>
+        <v>85000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3356,58 +3368,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3417,9 +3429,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3447,28 +3459,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3485,6 +3475,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3515,63 +3527,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3581,10 +3593,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3599,10 +3611,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>68</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3618,10 +3630,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>135</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3637,10 +3649,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>53</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3656,10 +3668,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>2</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3675,10 +3687,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>5</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3694,8 +3706,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3708,10 +3720,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3758,60 +3770,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="39" t="s">
@@ -3823,11 +3835,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3902,60 +3914,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3964,10 +3976,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +3994,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="35">
         <v>68</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4001,10 +4013,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="35">
         <v>135</v>
       </c>
-      <c r="F33" s="38"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4020,10 +4032,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="35">
         <v>53</v>
       </c>
-      <c r="F34" s="38"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4039,10 +4051,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="35">
         <v>2</v>
       </c>
-      <c r="F35" s="38"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4058,10 +4070,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="35">
         <v>5</v>
       </c>
-      <c r="F36" s="38"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4077,8 +4089,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4141,60 +4153,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="27"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40" t="s">
@@ -4206,11 +4218,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4238,30 +4250,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4278,6 +4266,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4309,63 +4321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4375,10 +4387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4393,10 +4405,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>44</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4412,10 +4424,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>118</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4431,10 +4443,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>510</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4450,8 +4462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4467,8 +4479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4484,8 +4496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4498,10 +4510,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4548,72 +4560,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4688,60 +4700,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4750,10 +4762,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4768,10 +4780,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="27">
         <v>44</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4787,10 +4799,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>118</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4806,10 +4818,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>510</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4825,8 +4837,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4842,8 +4854,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4859,8 +4871,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4873,10 +4885,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4923,58 +4935,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40"/>
@@ -4984,11 +4996,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5016,6 +5028,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5028,34 +5068,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5080,64 +5092,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5148,8 +5160,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5160,8 +5172,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5172,8 +5184,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5184,8 +5196,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5196,8 +5208,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5208,8 +5220,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5219,8 +5231,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5264,52 +5276,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5319,9 +5331,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5408,60 +5420,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5472,10 +5484,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5490,10 +5502,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>30</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5509,10 +5521,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>35</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5528,10 +5540,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="27">
         <v>425</v>
       </c>
-      <c r="F35" s="25"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5547,8 +5559,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5564,8 +5576,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5581,10 +5593,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="35">
         <v>100</v>
       </c>
-      <c r="F38" s="38"/>
+      <c r="F38" s="35"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5597,10 +5609,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5647,58 +5659,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5708,20 +5720,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5734,24 +5756,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5777,177 +5789,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="52">
+      <c r="A5" s="45">
         <v>1</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="51">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="52"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="51"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="52">
+      <c r="A7" s="45">
         <v>2</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="51">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="52"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="51"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="52">
+      <c r="A9" s="45">
         <v>3</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="51">
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="52"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="51"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="52">
+      <c r="A11" s="45">
         <v>4</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="51">
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="47">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="52"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="47"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="51">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="47">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="51"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5958,10 +5970,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -5976,8 +5988,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -5993,10 +6005,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="27">
         <v>30</v>
       </c>
-      <c r="F27" s="25"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6012,8 +6024,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6029,10 +6041,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="27">
         <v>5</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="27"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6048,8 +6060,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6065,10 +6077,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E31" s="35">
         <v>2</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6081,10 +6093,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6131,58 +6143,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="27" t="s">
+      <c r="H39" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6192,12 +6204,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="A13:F14"/>
     <mergeCell ref="H40:J40"/>
@@ -6214,23 +6243,6 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
11.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 10.07.19</t>
+    <t>Date: 11.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,11 +388,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -403,36 +430,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -440,6 +437,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,23 +451,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -486,6 +480,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>50</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>16</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>151</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>58</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>50</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>116</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>151</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>58</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,6 +2662,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2674,32 +2700,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2711,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
-        <v>22</v>
-      </c>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25">
+        <v>29</v>
+      </c>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>22000</v>
+        <v>29000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
-        <v>85</v>
-      </c>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25">
+        <v>110</v>
+      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>42500</v>
+        <v>55000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
-        <v>82</v>
-      </c>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25">
+        <v>281</v>
+      </c>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>8200</v>
+        <v>28100</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,13 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
-        <v>200</v>
-      </c>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25">
+        <v>106</v>
+      </c>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>5300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,13 +2890,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
-        <v>15</v>
-      </c>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25">
+        <v>22</v>
+      </c>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>440</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2909,13 +2909,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27">
-        <v>200</v>
-      </c>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25">
+        <v>16</v>
+      </c>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>160</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2925,14 +2925,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>85000</v>
+        <v>118000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2975,58 +2975,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3036,9 +3036,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3125,60 +3125,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3189,10 +3189,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -3207,13 +3207,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
-        <v>22</v>
-      </c>
-      <c r="F33" s="27"/>
+      <c r="E33" s="25">
+        <v>29</v>
+      </c>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>22000</v>
+        <v>29000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3226,13 +3226,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
-        <v>85</v>
-      </c>
-      <c r="F34" s="27"/>
+      <c r="E34" s="25">
+        <v>110</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>42500</v>
+        <v>55000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3245,13 +3245,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
-        <v>82</v>
-      </c>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25">
+        <v>281</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>8200</v>
+        <v>28100</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3264,13 +3264,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="27">
-        <v>200</v>
-      </c>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25">
+        <v>106</v>
+      </c>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>5300</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3283,13 +3283,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="35">
-        <v>15</v>
-      </c>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38">
+        <v>22</v>
+      </c>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>300</v>
+        <v>440</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3302,13 +3302,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
-        <v>200</v>
-      </c>
-      <c r="F38" s="35"/>
+      <c r="E38" s="38">
+        <v>16</v>
+      </c>
+      <c r="F38" s="38"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>160</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3318,14 +3318,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>85000</v>
+        <v>118000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3368,58 +3368,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3429,9 +3429,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3459,6 +3459,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3475,28 +3497,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3527,63 +3527,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3593,10 +3593,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3611,10 +3611,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>68</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3630,10 +3630,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>135</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3649,10 +3649,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>53</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3668,10 +3668,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>2</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3687,10 +3687,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3706,8 +3706,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3720,10 +3720,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3770,60 +3770,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="39" t="s">
@@ -3835,11 +3835,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3914,60 +3914,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3976,10 +3976,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3994,10 +3994,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="35">
+      <c r="E32" s="38">
         <v>68</v>
       </c>
-      <c r="F32" s="35"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4013,10 +4013,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="38">
         <v>135</v>
       </c>
-      <c r="F33" s="35"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4032,10 +4032,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E34" s="38">
         <v>53</v>
       </c>
-      <c r="F34" s="35"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4051,10 +4051,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="38">
         <v>2</v>
       </c>
-      <c r="F35" s="35"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4070,10 +4070,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="38">
         <v>5</v>
       </c>
-      <c r="F36" s="35"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4089,8 +4089,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4153,60 +4153,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40" t="s">
@@ -4218,11 +4218,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4250,6 +4250,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4266,30 +4290,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4321,63 +4321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4387,10 +4387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4405,10 +4405,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>44</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4424,10 +4424,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>118</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4443,10 +4443,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>510</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4462,8 +4462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4479,8 +4479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4496,8 +4496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4510,10 +4510,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4560,72 +4560,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4700,60 +4700,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4762,10 +4762,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4780,10 +4780,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4799,10 +4799,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>118</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4818,10 +4818,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>510</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4837,8 +4837,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4854,8 +4854,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4871,8 +4871,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4885,10 +4885,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4935,58 +4935,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40"/>
@@ -4996,11 +4996,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5028,16 +5028,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5050,24 +5058,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5092,64 +5092,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5160,8 +5160,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5172,8 +5172,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5184,8 +5184,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5196,8 +5196,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5208,8 +5208,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5220,8 +5220,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5231,8 +5231,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5276,52 +5276,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5331,9 +5331,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5420,60 +5420,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5484,10 +5484,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5502,10 +5502,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>30</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5521,10 +5521,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>35</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5540,10 +5540,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>425</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5559,8 +5559,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5576,8 +5576,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5593,10 +5593,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
+      <c r="E38" s="38">
         <v>100</v>
       </c>
-      <c r="F38" s="35"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5609,10 +5609,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5659,58 +5659,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5720,12 +5720,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5738,32 +5764,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5789,177 +5789,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="45">
+      <c r="A5" s="52">
         <v>1</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47">
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="44">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="45">
+      <c r="A7" s="52">
         <v>2</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="44">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="45">
+      <c r="A9" s="52">
         <v>3</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="47">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="44">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="47"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="45">
+      <c r="A11" s="52">
         <v>4</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="47">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="44">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="45"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="47"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="47">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="44">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="47"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5970,10 +5970,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -5988,8 +5988,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6005,10 +6005,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="25">
         <v>30</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6024,8 +6024,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6041,10 +6041,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <v>5</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6060,8 +6060,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6077,10 +6077,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="38">
         <v>2</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6093,10 +6093,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6143,58 +6143,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6204,31 +6204,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A13:F14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6243,6 +6224,25 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
14.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 11.07.19</t>
+    <t>Date: 14.07.19</t>
   </si>
 </sst>
 </file>
@@ -458,9 +458,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -480,6 +477,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2711,7 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
@@ -2815,12 +2815,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="25">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>29000</v>
+        <v>15000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2834,12 +2834,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="25">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2853,12 +2853,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="25">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>28100</v>
+        <v>28200</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2872,12 +2872,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="25">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>5300</v>
+        <v>7800</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,13 +2890,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25">
-        <v>22</v>
-      </c>
+      <c r="E10" s="25"/>
       <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>440</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2909,13 +2907,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25">
-        <v>16</v>
-      </c>
+      <c r="E11" s="25"/>
       <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2932,7 +2928,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>118000</v>
+        <v>101000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -3208,12 +3204,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="25">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>29000</v>
+        <v>15000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3227,12 +3223,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="25">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>55000</v>
+        <v>50000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3246,12 +3242,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="25">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>28100</v>
+        <v>28200</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3265,12 +3261,12 @@
         <v>50</v>
       </c>
       <c r="E36" s="25">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>5300</v>
+        <v>7800</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3283,13 +3279,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="38">
-        <v>22</v>
-      </c>
+      <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>440</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3302,13 +3296,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="38">
-        <v>16</v>
-      </c>
+      <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3325,7 +3317,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>118000</v>
+        <v>101000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -5820,97 +5812,97 @@
       <c r="A5" s="52">
         <v>1</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="44">
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="51">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="52"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="52">
         <v>2</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="44">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="51">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="52"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="52">
         <v>3</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="44">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="51">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="52"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="52">
         <v>4</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="44">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="51">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="52"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="44"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="53" t="s">
@@ -5921,7 +5913,7 @@
       <c r="D13" s="53"/>
       <c r="E13" s="53"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="44">
+      <c r="G13" s="51">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
@@ -5933,7 +5925,7 @@
       <c r="D14" s="53"/>
       <c r="E14" s="53"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="44"/>
+      <c r="G14" s="51"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
       <c r="A23" s="31" t="s">
@@ -6210,6 +6202,8 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6224,6 +6218,10 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6237,12 +6235,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
15.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 14.07.19</t>
+    <t>Date: 15.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,38 +388,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -430,6 +403,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -437,9 +440,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,11 +451,17 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -477,12 +483,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>50</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>16</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>151</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>58</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="27">
         <v>50</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>116</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>151</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="27">
         <v>58</v>
       </c>
-      <c r="F35" s="25"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,14 +2662,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2682,24 +2692,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
-        <v>15</v>
-      </c>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27">
+        <v>30</v>
+      </c>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>15000</v>
+        <v>30000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
-        <v>100</v>
-      </c>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27">
+        <v>157</v>
+      </c>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>78500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
-        <v>282</v>
-      </c>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27">
+        <v>52</v>
+      </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>28200</v>
+        <v>5200</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,13 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
-        <v>156</v>
-      </c>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27">
+        <v>138</v>
+      </c>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>7800</v>
+        <v>6900</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,11 +2890,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27">
+        <v>70</v>
+      </c>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2907,8 +2909,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2921,14 +2923,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>101000</v>
+        <v>122000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2971,58 +2973,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3032,9 +3034,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3121,60 +3123,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3185,10 +3187,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -3203,13 +3205,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="25">
-        <v>15</v>
-      </c>
-      <c r="F33" s="25"/>
+      <c r="E33" s="27">
+        <v>30</v>
+      </c>
+      <c r="F33" s="27"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>15000</v>
+        <v>30000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3222,13 +3224,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="25">
-        <v>100</v>
-      </c>
-      <c r="F34" s="25"/>
+      <c r="E34" s="27">
+        <v>157</v>
+      </c>
+      <c r="F34" s="27"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>50000</v>
+        <v>78500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3241,13 +3243,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
-        <v>282</v>
-      </c>
-      <c r="F35" s="25"/>
+      <c r="E35" s="27">
+        <v>52</v>
+      </c>
+      <c r="F35" s="27"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>28200</v>
+        <v>5200</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3260,13 +3262,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="25">
-        <v>156</v>
-      </c>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27">
+        <v>138</v>
+      </c>
+      <c r="F36" s="27"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>7800</v>
+        <v>6900</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3279,11 +3281,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="35">
+        <v>70</v>
+      </c>
+      <c r="F37" s="35"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3296,8 +3300,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3310,14 +3314,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>101000</v>
+        <v>122000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3360,58 +3364,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3421,9 +3425,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3451,28 +3455,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3489,6 +3471,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3519,63 +3523,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3585,10 +3589,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3603,10 +3607,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>68</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3622,10 +3626,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>135</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3641,10 +3645,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>53</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3660,10 +3664,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>2</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3679,10 +3683,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>5</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3698,8 +3702,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3712,10 +3716,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3762,60 +3766,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="39" t="s">
@@ -3827,11 +3831,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3906,60 +3910,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3968,10 +3972,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +3990,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="35">
         <v>68</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4005,10 +4009,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="35">
         <v>135</v>
       </c>
-      <c r="F33" s="38"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4024,10 +4028,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="35">
         <v>53</v>
       </c>
-      <c r="F34" s="38"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4043,10 +4047,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="35">
         <v>2</v>
       </c>
-      <c r="F35" s="38"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4062,10 +4066,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="35">
         <v>5</v>
       </c>
-      <c r="F36" s="38"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4081,8 +4085,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4145,60 +4149,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="27"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40" t="s">
@@ -4210,11 +4214,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4242,30 +4246,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4282,6 +4262,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4313,63 +4317,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4379,10 +4383,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4397,10 +4401,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>44</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4416,10 +4420,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>118</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4435,10 +4439,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>510</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4454,8 +4458,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4471,8 +4475,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4488,8 +4492,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4502,10 +4506,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4552,72 +4556,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4692,60 +4696,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4754,10 +4758,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4772,10 +4776,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="27">
         <v>44</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4791,10 +4795,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>118</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4810,10 +4814,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>510</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4829,8 +4833,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4846,8 +4850,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4863,8 +4867,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4877,10 +4881,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4927,58 +4931,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40"/>
@@ -4988,11 +4992,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5020,6 +5024,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5032,34 +5064,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5084,64 +5088,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5152,8 +5156,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5164,8 +5168,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5176,8 +5180,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5188,8 +5192,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5200,8 +5204,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5212,8 +5216,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5223,8 +5227,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5268,52 +5272,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5323,9 +5327,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5412,60 +5416,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5476,10 +5480,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5494,10 +5498,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>30</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5513,10 +5517,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>35</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5532,10 +5536,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="27">
         <v>425</v>
       </c>
-      <c r="F35" s="25"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5551,8 +5555,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5568,8 +5572,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5585,10 +5589,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="35">
         <v>100</v>
       </c>
-      <c r="F38" s="38"/>
+      <c r="F38" s="35"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5601,10 +5605,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="37"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5651,58 +5655,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5712,20 +5716,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5738,24 +5752,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5781,128 +5785,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="52">
+      <c r="A5" s="45">
         <v>1</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="51">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="44">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="52"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="51"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="52">
+      <c r="A7" s="45">
         <v>2</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="51">
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="44">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="52"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="51"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="44"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="52">
+      <c r="A9" s="45">
         <v>3</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="51">
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="44">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="52"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="51"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="52">
+      <c r="A11" s="45">
         <v>4</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="51">
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="44">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="52"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="44"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="53" t="s">
@@ -5913,7 +5917,7 @@
       <c r="D13" s="53"/>
       <c r="E13" s="53"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="51">
+      <c r="G13" s="44">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
@@ -5925,33 +5929,33 @@
       <c r="D14" s="53"/>
       <c r="E14" s="53"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="51"/>
+      <c r="G14" s="44"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5962,10 +5966,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -5980,8 +5984,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -5997,10 +6001,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="27">
         <v>30</v>
       </c>
-      <c r="F27" s="25"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6016,8 +6020,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6033,10 +6037,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="27">
         <v>5</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="27"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6052,8 +6056,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6069,10 +6073,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E31" s="35">
         <v>2</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6085,10 +6089,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6135,58 +6139,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="27" t="s">
+      <c r="H39" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6196,12 +6200,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
@@ -6218,23 +6239,6 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
17.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 15.07.19</t>
+    <t>Date: 17.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,11 +388,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -403,36 +430,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -440,6 +437,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,16 +451,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -484,7 +481,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>50</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>16</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>151</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>58</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>50</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>116</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>151</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>58</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,6 +2662,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2674,32 +2700,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2711,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
-        <v>30</v>
-      </c>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25">
+        <v>17</v>
+      </c>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
-        <v>157</v>
-      </c>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25">
+        <v>104</v>
+      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>78500</v>
+        <v>52000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
-        <v>52</v>
-      </c>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25">
+        <v>135</v>
+      </c>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>5200</v>
+        <v>13500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,13 +2871,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
-        <v>138</v>
-      </c>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>6900</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,13 +2888,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
-        <v>70</v>
-      </c>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25">
+        <v>25</v>
+      </c>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2909,8 +2907,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2923,14 +2921,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>122000</v>
+        <v>83000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2973,58 +2971,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3034,9 +3032,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3123,60 +3121,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3187,10 +3185,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -3205,13 +3203,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
-        <v>30</v>
-      </c>
-      <c r="F33" s="27"/>
+      <c r="E33" s="25">
+        <v>17</v>
+      </c>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3224,13 +3222,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
-        <v>157</v>
-      </c>
-      <c r="F34" s="27"/>
+      <c r="E34" s="25">
+        <v>104</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>78500</v>
+        <v>52000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3243,13 +3241,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
-        <v>52</v>
-      </c>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25">
+        <v>135</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>5200</v>
+        <v>13500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3262,13 +3260,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="27">
-        <v>138</v>
-      </c>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>6900</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3281,13 +3277,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="35">
-        <v>70</v>
-      </c>
-      <c r="F37" s="35"/>
+      <c r="E37" s="25">
+        <v>25</v>
+      </c>
+      <c r="F37" s="25"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3300,8 +3296,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3314,14 +3310,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>122000</v>
+        <v>83000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3364,58 +3360,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3425,9 +3421,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3455,6 +3451,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3471,28 +3489,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3523,63 +3519,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3589,10 +3585,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3607,10 +3603,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>68</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3626,10 +3622,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>135</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3645,10 +3641,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>53</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3664,10 +3660,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>2</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3683,10 +3679,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3702,8 +3698,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3716,10 +3712,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3766,60 +3762,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="39" t="s">
@@ -3831,11 +3827,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3910,60 +3906,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3972,10 +3968,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3990,10 +3986,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="35">
+      <c r="E32" s="38">
         <v>68</v>
       </c>
-      <c r="F32" s="35"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4009,10 +4005,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="38">
         <v>135</v>
       </c>
-      <c r="F33" s="35"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4028,10 +4024,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E34" s="38">
         <v>53</v>
       </c>
-      <c r="F34" s="35"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4047,10 +4043,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="35">
+      <c r="E35" s="38">
         <v>2</v>
       </c>
-      <c r="F35" s="35"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4066,10 +4062,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="38">
         <v>5</v>
       </c>
-      <c r="F36" s="35"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4085,8 +4081,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4149,60 +4145,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40" t="s">
@@ -4214,11 +4210,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4246,6 +4242,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4262,30 +4282,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4317,63 +4313,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4383,10 +4379,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4401,10 +4397,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>44</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4420,10 +4416,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>118</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4439,10 +4435,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>510</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4458,8 +4454,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4475,8 +4471,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4492,8 +4488,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4506,10 +4502,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4556,72 +4552,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4696,60 +4692,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4758,10 +4754,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4776,10 +4772,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4795,10 +4791,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>118</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4814,10 +4810,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>510</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4833,8 +4829,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4850,8 +4846,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4867,8 +4863,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4881,10 +4877,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4931,58 +4927,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="40"/>
@@ -4992,11 +4988,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5024,16 +5020,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5046,24 +5050,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5088,64 +5084,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5156,8 +5152,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5168,8 +5164,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5180,8 +5176,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5192,8 +5188,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5204,8 +5200,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5216,8 +5212,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5227,8 +5223,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5272,52 +5268,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5327,9 +5323,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5416,60 +5412,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5480,10 +5476,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5498,10 +5494,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>30</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5517,10 +5513,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>35</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5536,10 +5532,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>425</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5555,8 +5551,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5572,8 +5568,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5589,10 +5585,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="35">
+      <c r="E38" s="38">
         <v>100</v>
       </c>
-      <c r="F38" s="35"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5605,10 +5601,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="37"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5655,58 +5651,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5716,12 +5712,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5734,32 +5756,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5785,177 +5781,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="45">
+      <c r="A5" s="53">
         <v>1</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="44">
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="52">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="44"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="45">
+      <c r="A7" s="53">
         <v>2</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="44">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="52">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="44"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="52"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="45">
+      <c r="A9" s="53">
         <v>3</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="44">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="52">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="44"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="45">
+      <c r="A11" s="53">
         <v>4</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="44">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="52">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="45"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="44"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="52"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="44">
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="52">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="44"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="52"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5966,10 +5962,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -5984,8 +5980,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6001,10 +5997,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="25">
         <v>30</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6020,8 +6016,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6037,10 +6033,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <v>5</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6056,8 +6052,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6073,10 +6069,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="38">
         <v>2</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6089,10 +6085,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6139,58 +6135,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6200,31 +6196,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6239,6 +6216,25 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
18.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 17.07.19</t>
+    <t>Date: 18.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,38 +388,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -430,6 +403,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -437,9 +437,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,17 +448,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -481,10 +484,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>50</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>16</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>151</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>58</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="27">
         <v>50</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>116</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>151</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="27">
         <v>58</v>
       </c>
-      <c r="F35" s="25"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,14 +2662,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2682,24 +2692,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2712,7 +2712,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
-        <v>17</v>
-      </c>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27">
+        <v>115</v>
+      </c>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>17000</v>
+        <v>115000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
-        <v>104</v>
-      </c>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27">
+        <v>216</v>
+      </c>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>52000</v>
+        <v>108000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
-        <v>135</v>
-      </c>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27">
+        <v>400</v>
+      </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>13500</v>
+        <v>40000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,11 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27">
+        <v>6</v>
+      </c>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2888,13 +2890,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25">
-        <v>25</v>
-      </c>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2907,11 +2907,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27">
+        <v>70</v>
+      </c>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2921,14 +2923,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>83000</v>
+        <v>264000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2971,58 +2973,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3032,9 +3034,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3121,60 +3123,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3203,13 +3205,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="25">
-        <v>17</v>
-      </c>
-      <c r="F33" s="25"/>
+      <c r="E33" s="27">
+        <v>115</v>
+      </c>
+      <c r="F33" s="27"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>17000</v>
+        <v>115000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3222,13 +3224,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="25">
-        <v>104</v>
-      </c>
-      <c r="F34" s="25"/>
+      <c r="E34" s="27">
+        <v>216</v>
+      </c>
+      <c r="F34" s="27"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>52000</v>
+        <v>108000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3241,13 +3243,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
-        <v>135</v>
-      </c>
-      <c r="F35" s="25"/>
+      <c r="E35" s="27">
+        <v>400</v>
+      </c>
+      <c r="F35" s="27"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>13500</v>
+        <v>40000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3260,11 +3262,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27">
+        <v>6</v>
+      </c>
+      <c r="F36" s="27"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3277,13 +3281,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="25">
-        <v>25</v>
-      </c>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3296,11 +3298,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="E38" s="27">
+        <v>70</v>
+      </c>
+      <c r="F38" s="27"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3317,7 +3321,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>83000</v>
+        <v>264000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3360,58 +3364,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3421,9 +3425,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3451,28 +3455,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3489,6 +3471,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3519,63 +3523,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3585,10 +3589,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3603,10 +3607,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>68</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3622,10 +3626,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>135</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3641,10 +3645,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>53</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3660,10 +3664,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <v>2</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3679,10 +3683,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="27">
         <v>5</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3698,8 +3702,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3712,10 +3716,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3762,76 +3766,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="39"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3906,60 +3910,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3986,10 +3990,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="41">
         <v>68</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4005,10 +4009,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="41">
         <v>135</v>
       </c>
-      <c r="F33" s="38"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4024,10 +4028,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="41">
         <v>53</v>
       </c>
-      <c r="F34" s="38"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4043,10 +4047,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="41">
         <v>2</v>
       </c>
-      <c r="F35" s="38"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4062,10 +4066,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="41">
         <v>5</v>
       </c>
-      <c r="F36" s="38"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4081,8 +4085,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4095,10 +4099,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="41"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4145,76 +4149,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="27"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="40"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4242,30 +4246,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4282,6 +4262,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4313,63 +4317,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4379,10 +4383,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4397,10 +4401,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="27">
         <v>44</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4416,10 +4420,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="27">
         <v>118</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4435,10 +4439,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="27">
         <v>510</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4454,8 +4458,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4471,8 +4475,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4488,8 +4492,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4502,10 +4506,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4552,72 +4556,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4692,60 +4696,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4754,10 +4758,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4772,10 +4776,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="27">
         <v>44</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4791,10 +4795,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>118</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4810,10 +4814,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>510</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4829,8 +4833,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4846,8 +4850,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4863,8 +4867,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4877,10 +4881,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="43"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4927,72 +4931,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27" t="s">
+      <c r="H45" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5020,6 +5024,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5032,34 +5064,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5084,64 +5088,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5152,8 +5156,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5164,8 +5168,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5176,8 +5180,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5188,8 +5192,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5200,8 +5204,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5212,8 +5216,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5223,8 +5227,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5268,52 +5272,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5323,9 +5327,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5412,60 +5416,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5494,10 +5498,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="27">
         <v>30</v>
       </c>
-      <c r="F33" s="25"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5513,10 +5517,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="27">
         <v>35</v>
       </c>
-      <c r="F34" s="25"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5532,10 +5536,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="27">
         <v>425</v>
       </c>
-      <c r="F35" s="25"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5551,8 +5555,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5568,8 +5572,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5585,10 +5589,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="41">
         <v>100</v>
       </c>
-      <c r="F38" s="38"/>
+      <c r="F38" s="41"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5651,58 +5655,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5712,20 +5716,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5738,24 +5752,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5781,35 +5785,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="53">
+      <c r="A5" s="44">
         <v>1</v>
       </c>
       <c r="B5" s="45" t="s">
@@ -5819,21 +5823,21 @@
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
-      <c r="G5" s="52">
+      <c r="G5" s="46">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="53"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="52"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="53">
+      <c r="A7" s="44">
         <v>2</v>
       </c>
       <c r="B7" s="45" t="s">
@@ -5843,21 +5847,21 @@
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
       <c r="F7" s="45"/>
-      <c r="G7" s="52">
+      <c r="G7" s="46">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="53"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
       <c r="F8" s="45"/>
-      <c r="G8" s="52"/>
+      <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="53">
+      <c r="A9" s="44">
         <v>3</v>
       </c>
       <c r="B9" s="45" t="s">
@@ -5867,91 +5871,91 @@
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
       <c r="F9" s="45"/>
-      <c r="G9" s="52">
+      <c r="G9" s="46">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="53"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
       <c r="F10" s="45"/>
-      <c r="G10" s="52"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="53">
+      <c r="A11" s="44">
         <v>4</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="52">
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="46">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="53"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="46"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="52">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="46">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="52"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="46"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5980,8 +5984,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -5997,10 +6001,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="27">
         <v>30</v>
       </c>
-      <c r="F27" s="25"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6016,8 +6020,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6033,10 +6037,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="27">
         <v>5</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="27"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6052,8 +6056,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6069,10 +6073,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E31" s="41">
         <v>2</v>
       </c>
-      <c r="F31" s="38"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6135,58 +6139,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="27" t="s">
+      <c r="H39" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6196,12 +6200,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:F14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6216,25 +6237,8 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:F14"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
20.07.19 Today sales details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 18.07.19</t>
+    <t>Date: 20.07.19</t>
   </si>
 </sst>
 </file>
@@ -388,11 +388,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -402,33 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -451,20 +451,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -483,6 +477,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1933,7 +1933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +1955,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2017,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2035,10 +2035,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>50</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2054,10 +2054,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>16</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2073,10 +2073,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>151</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2092,10 +2092,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>58</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2111,8 +2111,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2128,8 +2128,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2142,10 +2142,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2192,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2253,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2332,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2394,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2412,10 +2412,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>50</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2431,10 +2431,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>116</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2450,10 +2450,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>151</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2469,10 +2469,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>58</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2488,8 +2488,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2505,8 +2505,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2519,10 +2519,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2569,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2630,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,6 +2662,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2674,32 +2700,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2730,63 +2730,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2796,10 +2796,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2814,13 +2814,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
-        <v>115</v>
-      </c>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25">
+        <v>34</v>
+      </c>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>115000</v>
+        <v>34000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2833,13 +2833,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
-        <v>216</v>
-      </c>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25">
+        <v>133</v>
+      </c>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>108000</v>
+        <v>66500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2852,13 +2852,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
-        <v>400</v>
-      </c>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25">
+        <v>684</v>
+      </c>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>68400</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2871,13 +2871,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
-        <v>6</v>
-      </c>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25">
+        <v>72</v>
+      </c>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2890,11 +2890,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25">
+        <v>75</v>
+      </c>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2907,13 +2909,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27">
-        <v>70</v>
-      </c>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25">
+        <v>100</v>
+      </c>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2923,14 +2925,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>264000</v>
+        <v>175000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2973,58 +2975,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -3034,9 +3036,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3123,60 +3125,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -3205,13 +3207,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
-        <v>115</v>
-      </c>
-      <c r="F33" s="27"/>
+      <c r="E33" s="25">
+        <v>34</v>
+      </c>
+      <c r="F33" s="25"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>115000</v>
+        <v>34000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -3224,13 +3226,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
-        <v>216</v>
-      </c>
-      <c r="F34" s="27"/>
+      <c r="E34" s="25">
+        <v>133</v>
+      </c>
+      <c r="F34" s="25"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>108000</v>
+        <v>66500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -3243,13 +3245,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
-        <v>400</v>
-      </c>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25">
+        <v>684</v>
+      </c>
+      <c r="F35" s="25"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>68400</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -3262,13 +3264,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="27">
-        <v>6</v>
-      </c>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25">
+        <v>72</v>
+      </c>
+      <c r="F36" s="25"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>3600</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -3281,11 +3283,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25">
+        <v>75</v>
+      </c>
+      <c r="F37" s="25"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -3298,13 +3302,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="27">
-        <v>70</v>
-      </c>
-      <c r="F38" s="27"/>
+      <c r="E38" s="25">
+        <v>100</v>
+      </c>
+      <c r="F38" s="25"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -3321,7 +3325,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>264000</v>
+        <v>175000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -3364,58 +3368,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3425,9 +3429,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3455,6 +3459,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3471,28 +3497,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3523,63 +3527,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3589,10 +3593,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3607,10 +3611,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>68</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3626,10 +3630,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>135</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3645,10 +3649,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>53</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3664,10 +3668,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <v>2</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3683,10 +3687,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3702,8 +3706,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3716,10 +3720,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3766,60 +3770,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="38" t="s">
@@ -3831,11 +3835,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3910,60 +3914,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4149,60 +4153,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="39" t="s">
@@ -4214,11 +4218,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4246,6 +4250,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4262,30 +4290,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4317,63 +4321,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4383,10 +4387,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4401,10 +4405,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <v>44</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4420,10 +4424,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <v>118</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4439,10 +4443,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <v>510</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4458,8 +4462,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4475,8 +4479,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4492,8 +4496,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4506,10 +4510,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4556,72 +4560,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4696,60 +4700,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4758,10 +4762,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4776,10 +4780,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4795,10 +4799,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>118</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4814,10 +4818,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>510</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4833,8 +4837,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4850,8 +4854,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4867,8 +4871,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4881,10 +4885,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4931,58 +4935,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="39"/>
@@ -4992,11 +4996,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5024,16 +5028,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5046,24 +5058,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5088,64 +5092,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5156,8 +5160,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5168,8 +5172,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5180,8 +5184,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5192,8 +5196,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5204,8 +5208,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5216,8 +5220,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5227,8 +5231,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5272,52 +5276,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5327,9 +5331,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5416,60 +5420,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5498,10 +5502,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <v>30</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5517,10 +5521,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <v>35</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5536,10 +5540,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="25">
         <v>425</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5555,8 +5559,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5655,58 +5659,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5716,12 +5720,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5734,32 +5764,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5785,128 +5789,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="44">
+      <c r="A5" s="52">
         <v>1</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="46">
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="51">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="44">
+      <c r="A7" s="52">
         <v>2</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="51">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="51"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="44">
+      <c r="A9" s="52">
         <v>3</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="51">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="44">
+      <c r="A11" s="52">
         <v>4</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="46">
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="51">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="44"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="46"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="53" t="s">
@@ -5917,7 +5921,7 @@
       <c r="D13" s="53"/>
       <c r="E13" s="53"/>
       <c r="F13" s="53"/>
-      <c r="G13" s="46">
+      <c r="G13" s="51">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
@@ -5929,33 +5933,33 @@
       <c r="D14" s="53"/>
       <c r="E14" s="53"/>
       <c r="F14" s="53"/>
-      <c r="G14" s="46"/>
+      <c r="G14" s="51"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5984,8 +5988,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6001,10 +6005,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="25">
         <v>30</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6020,8 +6024,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6037,10 +6041,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <v>5</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6139,58 +6143,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6200,12 +6204,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
@@ -6222,23 +6243,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
24.07.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,14 +101,14 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 21.07.19</t>
+    <t>Date: 24.07.19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +207,52 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -338,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -388,12 +434,45 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -403,33 +482,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -451,41 +503,102 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1933,7 +2046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1955,60 +2068,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2017,10 +2130,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2142,10 +2255,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2192,58 +2305,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2253,11 +2366,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2332,60 +2445,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2394,10 +2507,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2519,10 +2632,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="35"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2569,58 +2682,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2630,11 +2743,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2662,6 +2775,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2674,32 +2813,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2711,8 +2824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2730,688 +2843,681 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="8" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="60"/>
+      <c r="G5" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="61">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
-        <v>71</v>
-      </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="3">
+      <c r="E6" s="62">
+        <v>6</v>
+      </c>
+      <c r="F6" s="62"/>
+      <c r="G6" s="61">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>71000</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+        <v>6000</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="61">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
-        <v>158</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="3">
+      <c r="E7" s="62">
+        <v>51</v>
+      </c>
+      <c r="F7" s="62"/>
+      <c r="G7" s="61">
         <f t="shared" si="0"/>
-        <v>79000</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+        <v>25500</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="61">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
-        <v>200</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="3">
+      <c r="E8" s="62">
+        <v>85</v>
+      </c>
+      <c r="F8" s="62"/>
+      <c r="G8" s="61">
         <f t="shared" si="0"/>
-        <v>20000</v>
-      </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+        <v>8500</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="61">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="62">
+        <v>12</v>
+      </c>
+      <c r="F9" s="62"/>
+      <c r="G9" s="61">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" ht="27.95" customHeight="1">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="61">
+        <v>20</v>
+      </c>
+      <c r="E10" s="62">
+        <v>320</v>
+      </c>
+      <c r="F10" s="62"/>
+      <c r="G10" s="61">
+        <f t="shared" si="0"/>
+        <v>6400</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" ht="27.95" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="61">
+        <v>10</v>
+      </c>
+      <c r="E11" s="62">
         <v>100</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="3">
+      <c r="F11" s="62"/>
+      <c r="G11" s="61">
         <f t="shared" si="0"/>
-        <v>5000</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="27.95" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="60"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="21">
+        <f>SUM(G6:G11)</f>
+        <v>48000</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="63" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="63"/>
+      <c r="J16" s="63"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="63"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A19" s="65"/>
+      <c r="B19" s="65"/>
+      <c r="H19" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="68"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" ht="37.5" customHeight="1">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" ht="31.5">
+      <c r="A28" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+    </row>
+    <row r="29" spans="1:10" ht="18">
+      <c r="A29" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="57"/>
+    </row>
+    <row r="30" spans="1:10" ht="18.75">
+      <c r="A30" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+    </row>
+    <row r="31" spans="1:10" ht="40.5" customHeight="1">
+      <c r="A31" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+    </row>
+    <row r="32" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="71"/>
+      <c r="G32" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="72">
+        <v>1000</v>
+      </c>
+      <c r="E33" s="62">
+        <v>6</v>
+      </c>
+      <c r="F33" s="62"/>
+      <c r="G33" s="72">
+        <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
+        <v>6000</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="72">
+        <v>500</v>
+      </c>
+      <c r="E34" s="62">
+        <v>51</v>
+      </c>
+      <c r="F34" s="62"/>
+      <c r="G34" s="72">
+        <f t="shared" si="1"/>
+        <v>25500</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="72">
+        <v>100</v>
+      </c>
+      <c r="E35" s="62">
+        <v>85</v>
+      </c>
+      <c r="F35" s="62"/>
+      <c r="G35" s="72">
+        <f t="shared" si="1"/>
+        <v>8500</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="72">
+        <v>50</v>
+      </c>
+      <c r="E36" s="62">
+        <v>12</v>
+      </c>
+      <c r="F36" s="62"/>
+      <c r="G36" s="72">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="72">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="3">
+      <c r="E37" s="62">
+        <v>320</v>
+      </c>
+      <c r="F37" s="62"/>
+      <c r="G37" s="72">
+        <f>SUM(D37*E37)</f>
+        <v>6400</v>
+      </c>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="72">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="27.95" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8">
-        <f>SUM(G6:G11)</f>
-        <v>175000</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="E38" s="62">
+        <v>100</v>
+      </c>
+      <c r="F38" s="62"/>
+      <c r="G38" s="72">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" ht="27.95" customHeight="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="74"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="22">
+        <f>SUM(G33:G38)</f>
+        <v>48000</v>
+      </c>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
+      <c r="A43" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="B43" s="75"/>
+      <c r="H43" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="I43" s="75"/>
+      <c r="J43" s="75"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="65"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="65"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="65"/>
+      <c r="J45" s="65"/>
+    </row>
+    <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
+      <c r="A46" s="65"/>
+      <c r="B46" s="65"/>
+      <c r="H46" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" ht="37.5" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-    </row>
-    <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-    </row>
-    <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-    </row>
-    <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-    </row>
-    <row r="32" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E33" s="27">
-        <v>71</v>
-      </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="2">
-        <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>71000</v>
-      </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="2">
-        <v>500</v>
-      </c>
-      <c r="E34" s="27">
-        <v>158</v>
-      </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="2">
-        <f t="shared" si="1"/>
-        <v>79000</v>
-      </c>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="2">
-        <v>100</v>
-      </c>
-      <c r="E35" s="27">
-        <v>200</v>
-      </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="2">
-        <f t="shared" si="1"/>
-        <v>20000</v>
-      </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="2">
-        <v>50</v>
-      </c>
-      <c r="E36" s="27">
-        <v>100</v>
-      </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="2">
-        <f t="shared" si="1"/>
-        <v>5000</v>
-      </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="2">
-        <v>20</v>
-      </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="2">
-        <f>SUM(D37*E37)</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="2">
-        <v>10</v>
-      </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9">
-        <f>SUM(G33:G38)</f>
-        <v>175000</v>
-      </c>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-    </row>
-    <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="75"/>
+      <c r="J46" s="75"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3421,9 +3527,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3451,6 +3557,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3467,28 +3595,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3519,63 +3625,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3585,10 +3691,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3712,10 +3818,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3762,76 +3868,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3906,60 +4012,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3968,10 +4074,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="37" t="s">
+      <c r="E31" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="37"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3986,10 +4092,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="43">
         <v>68</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4005,10 +4111,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="43">
         <v>135</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4024,10 +4130,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="43">
         <v>53</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="43"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4043,10 +4149,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="43">
         <v>2</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="43"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4062,10 +4168,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="41">
+      <c r="E36" s="43">
         <v>5</v>
       </c>
-      <c r="F36" s="41"/>
+      <c r="F36" s="43"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4081,8 +4187,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4095,10 +4201,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4145,76 +4251,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="26"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="39"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4242,6 +4348,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4258,30 +4388,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4313,63 +4419,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4379,10 +4485,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4502,10 +4608,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4552,72 +4658,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="42"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="45"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4692,60 +4798,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4754,10 +4860,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="32"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4877,10 +4983,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="43" t="s">
+      <c r="D38" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="44"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4927,72 +5033,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="36"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="25" t="s">
+      <c r="H42" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26" t="s">
+      <c r="H45" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5020,16 +5126,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5042,24 +5156,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5084,64 +5190,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5223,8 +5329,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5268,52 +5374,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5323,9 +5429,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5412,60 +5518,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5476,10 +5582,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5568,8 +5674,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5585,10 +5691,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="41">
+      <c r="E38" s="43">
         <v>100</v>
       </c>
-      <c r="F38" s="41"/>
+      <c r="F38" s="43"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5601,10 +5707,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="36"/>
+      <c r="E39" s="38"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5651,58 +5757,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="25"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="26" t="s">
+      <c r="H46" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5712,12 +5818,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="22"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5730,32 +5862,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5781,107 +5887,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="45">
+      <c r="A5" s="54">
         <v>1</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="46">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="45">
+      <c r="A7" s="54">
         <v>2</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="46">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="45"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="45">
+      <c r="A9" s="54">
         <v>3</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="47">
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="46">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="45"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="47"/>
+      <c r="A10" s="54"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="45">
+      <c r="A11" s="54">
         <v>4</v>
       </c>
       <c r="B11" s="48" t="s">
@@ -5891,67 +5997,67 @@
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
       <c r="F11" s="50"/>
-      <c r="G11" s="47">
+      <c r="G11" s="46">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="45"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="51"/>
       <c r="C12" s="52"/>
       <c r="D12" s="52"/>
       <c r="E12" s="52"/>
       <c r="F12" s="53"/>
-      <c r="G12" s="47"/>
+      <c r="G12" s="46"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="47">
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="46">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="44"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="47"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="46"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -5962,10 +6068,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6052,8 +6158,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6069,10 +6175,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E31" s="43">
         <v>2</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="43"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6085,10 +6191,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="36"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6135,58 +6241,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6196,31 +6302,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="A13:F14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6235,6 +6322,25 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
25.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 24.07.19</t>
+    <t>Date: 25.07.19</t>
   </si>
 </sst>
 </file>
@@ -440,47 +440,123 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -488,33 +564,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -533,72 +591,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2046,7 +2046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2068,60 +2068,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2130,10 +2130,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2148,10 +2148,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2167,10 +2167,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2186,10 +2186,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2205,10 +2205,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2224,8 +2224,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2241,8 +2241,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2255,10 +2255,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2305,58 +2305,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2366,11 +2366,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2445,60 +2445,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2507,10 +2507,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="23"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2525,10 +2525,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2544,10 +2544,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2563,10 +2563,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2582,10 +2582,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2601,8 +2601,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2618,8 +2618,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2632,10 +2632,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="35"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2682,58 +2682,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="36"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2743,11 +2743,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="31" t="s">
+      <c r="H46" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2775,14 +2775,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2795,24 +2805,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2825,7 +2825,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2843,77 +2843,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="59" t="s">
+      <c r="F5" s="46"/>
+      <c r="G5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="4"/>
@@ -2924,16 +2924,16 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="61">
+      <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="62">
-        <v>6</v>
-      </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="61">
+      <c r="E6" s="42">
+        <v>52</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>6000</v>
+        <v>52000</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2943,16 +2943,16 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="61">
+      <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="62">
-        <v>51</v>
-      </c>
-      <c r="F7" s="62"/>
-      <c r="G7" s="61">
+      <c r="E7" s="42">
+        <v>381</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>25500</v>
+        <v>190500</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2962,16 +2962,16 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="61">
+      <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="62">
-        <v>85</v>
-      </c>
-      <c r="F8" s="62"/>
-      <c r="G8" s="61">
+      <c r="E8" s="42">
+        <v>155</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>8500</v>
+        <v>15500</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2981,16 +2981,16 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="61">
+      <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="62">
-        <v>12</v>
-      </c>
-      <c r="F9" s="62"/>
-      <c r="G9" s="61">
+      <c r="E9" s="42">
+        <v>80</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>4000</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -3000,16 +3000,16 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="61">
+      <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="62">
-        <v>320</v>
-      </c>
-      <c r="F10" s="62"/>
-      <c r="G10" s="61">
+      <c r="E10" s="42">
+        <v>200</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>6400</v>
+        <v>4000</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3019,14 +3019,14 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="61">
+      <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="62">
+      <c r="E11" s="42">
         <v>100</v>
       </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="61">
+      <c r="F11" s="42"/>
+      <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
@@ -3038,14 +3038,14 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="60"/>
-      <c r="F12" s="59"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="21">
         <f>SUM(G6:G11)</f>
-        <v>48000</v>
+        <v>267000</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3088,53 +3088,53 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="63" t="s">
+      <c r="B16" s="47"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="63"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="65"/>
-      <c r="B19" s="65"/>
-      <c r="H19" s="66" t="s">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="H19" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="66"/>
-      <c r="J19" s="66"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4"/>
@@ -3144,9 +3144,9 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4"/>
@@ -3233,60 +3233,60 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-      <c r="J29" s="57"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="4" t="s">
@@ -3294,14 +3294,14 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="70" t="s">
+      <c r="D32" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="71" t="s">
+      <c r="E32" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="71"/>
-      <c r="G32" s="70" t="s">
+      <c r="F32" s="55"/>
+      <c r="G32" s="26" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="4"/>
@@ -3312,16 +3312,16 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="72">
+      <c r="D33" s="27">
         <v>1000</v>
       </c>
-      <c r="E33" s="62">
-        <v>6</v>
-      </c>
-      <c r="F33" s="62"/>
-      <c r="G33" s="72">
+      <c r="E33" s="42">
+        <v>52</v>
+      </c>
+      <c r="F33" s="42"/>
+      <c r="G33" s="27">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>6000</v>
+        <v>52000</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -3331,16 +3331,16 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="72">
+      <c r="D34" s="27">
         <v>500</v>
       </c>
-      <c r="E34" s="62">
-        <v>51</v>
-      </c>
-      <c r="F34" s="62"/>
-      <c r="G34" s="72">
+      <c r="E34" s="42">
+        <v>381</v>
+      </c>
+      <c r="F34" s="42"/>
+      <c r="G34" s="27">
         <f t="shared" si="1"/>
-        <v>25500</v>
+        <v>190500</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -3350,16 +3350,16 @@
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="72">
+      <c r="D35" s="27">
         <v>100</v>
       </c>
-      <c r="E35" s="62">
-        <v>85</v>
-      </c>
-      <c r="F35" s="62"/>
-      <c r="G35" s="72">
+      <c r="E35" s="42">
+        <v>155</v>
+      </c>
+      <c r="F35" s="42"/>
+      <c r="G35" s="27">
         <f t="shared" si="1"/>
-        <v>8500</v>
+        <v>15500</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3369,16 +3369,16 @@
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="72">
+      <c r="D36" s="27">
         <v>50</v>
       </c>
-      <c r="E36" s="62">
-        <v>12</v>
-      </c>
-      <c r="F36" s="62"/>
-      <c r="G36" s="72">
+      <c r="E36" s="42">
+        <v>80</v>
+      </c>
+      <c r="F36" s="42"/>
+      <c r="G36" s="27">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>4000</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -3388,16 +3388,16 @@
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="72">
+      <c r="D37" s="27">
         <v>20</v>
       </c>
-      <c r="E37" s="62">
-        <v>320</v>
-      </c>
-      <c r="F37" s="62"/>
-      <c r="G37" s="72">
+      <c r="E37" s="42">
+        <v>200</v>
+      </c>
+      <c r="F37" s="42"/>
+      <c r="G37" s="27">
         <f>SUM(D37*E37)</f>
-        <v>6400</v>
+        <v>4000</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -3407,14 +3407,14 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="72">
+      <c r="D38" s="27">
         <v>10</v>
       </c>
-      <c r="E38" s="62">
+      <c r="E38" s="42">
         <v>100</v>
       </c>
-      <c r="F38" s="62"/>
-      <c r="G38" s="72">
+      <c r="F38" s="42"/>
+      <c r="G38" s="27">
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
@@ -3426,14 +3426,14 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="73" t="s">
+      <c r="D39" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="74"/>
-      <c r="F39" s="70"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>48000</v>
+        <v>267000</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -3476,48 +3476,48 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="75" t="s">
+      <c r="A43" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="H43" s="75" t="s">
+      <c r="B43" s="52"/>
+      <c r="H43" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="75"/>
-      <c r="J43" s="75"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="65"/>
-      <c r="B44" s="65"/>
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="65"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="65"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="65"/>
-      <c r="B45" s="65"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="65"/>
-      <c r="I45" s="65"/>
-      <c r="J45" s="65"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="65"/>
-      <c r="B46" s="65"/>
-      <c r="H46" s="76" t="s">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="H46" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3527,9 +3527,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3557,28 +3557,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3595,6 +3573,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3625,63 +3625,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3691,10 +3691,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3709,10 +3709,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3728,10 +3728,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3747,10 +3747,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3766,10 +3766,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3785,10 +3785,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="27"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3804,8 +3804,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3818,10 +3818,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3868,76 +3868,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4012,60 +4012,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4074,10 +4074,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4092,10 +4092,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="43"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4111,10 +4111,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="43"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4130,10 +4130,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4149,10 +4149,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="43"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4168,10 +4168,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="43"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4187,8 +4187,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4201,10 +4201,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4251,76 +4251,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="36"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="41"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="31" t="s">
+      <c r="H46" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4348,30 +4348,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4388,6 +4364,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4419,63 +4419,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4485,10 +4485,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4503,10 +4503,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4522,10 +4522,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4541,10 +4541,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4560,8 +4560,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4577,8 +4577,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4594,8 +4594,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4608,10 +4608,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4658,72 +4658,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="45"/>
-      <c r="B20" s="45"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4798,60 +4798,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4860,10 +4860,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="23"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4878,10 +4878,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4897,10 +4897,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4916,10 +4916,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4935,8 +4935,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4952,8 +4952,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4969,8 +4969,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4983,10 +4983,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5033,72 +5033,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="36"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="29"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="29" t="s">
+      <c r="H45" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="31" t="s">
+      <c r="H46" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5126,6 +5126,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5138,34 +5166,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5190,64 +5190,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5258,8 +5258,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5270,8 +5270,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5282,8 +5282,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5294,8 +5294,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5306,8 +5306,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5318,8 +5318,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5329,8 +5329,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5374,52 +5374,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5429,9 +5429,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5518,60 +5518,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5582,10 +5582,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="39" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5600,10 +5600,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5619,10 +5619,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5638,10 +5638,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="27">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5657,8 +5657,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5674,8 +5674,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5691,10 +5691,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="43"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5707,10 +5707,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="38"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5757,58 +5757,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="36"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="36" t="s">
+      <c r="H43" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5818,20 +5818,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5844,24 +5854,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5887,177 +5887,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="54">
+      <c r="A5" s="65">
         <v>1</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="46">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="67">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="54"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="46"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="67"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="54">
+      <c r="A7" s="65">
         <v>2</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="46">
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="67">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="54"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="46"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="54">
+      <c r="A9" s="65">
         <v>3</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="46">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="54"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="46"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="54">
+      <c r="A11" s="65">
         <v>4</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="46">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="67">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="54"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="46"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="46">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="67">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="46"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="67"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6068,10 +6068,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="39"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6086,8 +6086,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6103,10 +6103,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6122,8 +6122,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6139,10 +6139,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="27"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6158,8 +6158,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6175,10 +6175,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="43"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6191,10 +6191,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="38"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6241,58 +6241,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="36"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="36" t="s">
+      <c r="H36" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="29"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-      <c r="J38" s="29"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="29" t="s">
+      <c r="H39" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6302,12 +6302,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:F6"/>
@@ -6322,25 +6339,8 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
27.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 25.07.19</t>
+    <t>Date: 27.07.19</t>
   </si>
 </sst>
 </file>
@@ -255,7 +255,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,130 +440,112 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -565,39 +553,57 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2046,7 +2052,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2068,60 +2074,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2130,10 +2136,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2148,10 +2154,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="28">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2167,10 +2173,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="28">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2186,10 +2192,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="28">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2205,10 +2211,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="28">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2224,8 +2230,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2241,8 +2247,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2255,10 +2261,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2305,58 +2311,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2366,11 +2372,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2445,60 +2451,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2507,10 +2513,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2525,10 +2531,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="28">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2544,10 +2550,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="28">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2563,10 +2569,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="28">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2582,10 +2588,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="28">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2601,8 +2607,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2618,8 +2624,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2632,10 +2638,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="36"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2682,58 +2688,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2743,11 +2749,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2775,6 +2781,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2787,32 +2819,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2825,7 +2831,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+      <selection activeCell="K47" sqref="A1:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2888,32 +2894,32 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="23" t="s">
+      <c r="F5" s="75"/>
+      <c r="G5" s="74" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="4"/>
@@ -2924,16 +2930,16 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>1000</v>
       </c>
-      <c r="E6" s="42">
-        <v>52</v>
-      </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="24">
+      <c r="E6" s="47">
+        <v>60</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="21">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>52000</v>
+        <v>60000</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2943,16 +2949,16 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <v>500</v>
       </c>
-      <c r="E7" s="42">
-        <v>381</v>
-      </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="24">
+      <c r="E7" s="47">
+        <v>340</v>
+      </c>
+      <c r="F7" s="47"/>
+      <c r="G7" s="21">
         <f t="shared" si="0"/>
-        <v>190500</v>
+        <v>170000</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2962,16 +2968,16 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>100</v>
       </c>
-      <c r="E8" s="42">
-        <v>155</v>
-      </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="24">
+      <c r="E8" s="47">
+        <v>400</v>
+      </c>
+      <c r="F8" s="47"/>
+      <c r="G8" s="21">
         <f t="shared" si="0"/>
-        <v>15500</v>
+        <v>40000</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2981,16 +2987,14 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>50</v>
       </c>
-      <c r="E9" s="42">
-        <v>80</v>
-      </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="24">
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="21">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -3000,16 +3004,14 @@
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>20</v>
       </c>
-      <c r="E10" s="42">
-        <v>200</v>
-      </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="24">
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="21">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3019,16 +3021,14 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>10</v>
       </c>
-      <c r="E11" s="42">
-        <v>100</v>
-      </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="24">
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="21">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -3038,14 +3038,14 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="21">
+      <c r="E12" s="75"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="76">
         <f>SUM(G6:G11)</f>
-        <v>267000</v>
+        <v>270000</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3088,48 +3088,48 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="47" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="H19" s="49" t="s">
         <v>12</v>
       </c>
@@ -3144,9 +3144,9 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4"/>
@@ -3261,32 +3261,32 @@
       <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="4" t="s">
@@ -3294,14 +3294,14 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="55"/>
-      <c r="G32" s="26" t="s">
+      <c r="F32" s="70"/>
+      <c r="G32" s="69" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="4"/>
@@ -3312,16 +3312,16 @@
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="27">
+      <c r="D33" s="23">
         <v>1000</v>
       </c>
-      <c r="E33" s="42">
-        <v>52</v>
-      </c>
-      <c r="F33" s="42"/>
-      <c r="G33" s="27">
+      <c r="E33" s="47">
+        <v>60</v>
+      </c>
+      <c r="F33" s="47"/>
+      <c r="G33" s="23">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>52000</v>
+        <v>60000</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -3331,16 +3331,16 @@
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="27">
+      <c r="D34" s="23">
         <v>500</v>
       </c>
-      <c r="E34" s="42">
-        <v>381</v>
-      </c>
-      <c r="F34" s="42"/>
-      <c r="G34" s="27">
+      <c r="E34" s="47">
+        <v>340</v>
+      </c>
+      <c r="F34" s="47"/>
+      <c r="G34" s="23">
         <f t="shared" si="1"/>
-        <v>190500</v>
+        <v>170000</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -3350,16 +3350,16 @@
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="27">
+      <c r="D35" s="23">
         <v>100</v>
       </c>
-      <c r="E35" s="42">
-        <v>155</v>
-      </c>
-      <c r="F35" s="42"/>
-      <c r="G35" s="27">
+      <c r="E35" s="47">
+        <v>400</v>
+      </c>
+      <c r="F35" s="47"/>
+      <c r="G35" s="23">
         <f t="shared" si="1"/>
-        <v>15500</v>
+        <v>40000</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3369,16 +3369,14 @@
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="27">
+      <c r="D36" s="23">
         <v>50</v>
       </c>
-      <c r="E36" s="42">
-        <v>80</v>
-      </c>
-      <c r="F36" s="42"/>
-      <c r="G36" s="27">
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="23">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -3388,16 +3386,14 @@
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="27">
+      <c r="D37" s="23">
         <v>20</v>
       </c>
-      <c r="E37" s="42">
-        <v>200</v>
-      </c>
-      <c r="F37" s="42"/>
-      <c r="G37" s="27">
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="23">
         <f>SUM(D37*E37)</f>
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -3407,16 +3403,14 @@
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="27">
+      <c r="D38" s="23">
         <v>10</v>
       </c>
-      <c r="E38" s="42">
-        <v>100</v>
-      </c>
-      <c r="F38" s="42"/>
-      <c r="G38" s="27">
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="23">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -3426,14 +3420,14 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="75" t="s">
+      <c r="D39" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="76"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="22">
+      <c r="E39" s="72"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="73">
         <f>SUM(G33:G38)</f>
-        <v>267000</v>
+        <v>270000</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -3476,48 +3470,48 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="52" t="s">
+      <c r="A43" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="52"/>
-      <c r="H43" s="52" t="s">
+      <c r="B43" s="40"/>
+      <c r="H43" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
-      <c r="H46" s="53" t="s">
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
+      <c r="H46" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3527,9 +3521,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3557,6 +3551,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3573,28 +3589,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3625,63 +3619,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3691,10 +3685,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3709,10 +3703,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="28">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3728,10 +3722,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="28">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3747,10 +3741,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="28">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3766,10 +3760,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="28">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3785,10 +3779,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="28">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3804,8 +3798,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3818,10 +3812,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3868,76 +3862,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4012,60 +4006,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4074,10 +4068,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="54"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4092,10 +4086,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="53">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4111,10 +4105,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="53">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="53"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4130,10 +4124,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="53">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="53"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4149,10 +4143,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="53">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="53"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4168,10 +4162,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="53">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="53"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4187,8 +4181,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4201,10 +4195,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="52"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4251,76 +4245,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4348,6 +4342,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4364,30 +4382,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4419,63 +4413,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4485,10 +4479,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4503,10 +4497,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="28">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4522,10 +4516,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="28">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4541,10 +4535,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="28">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4560,8 +4554,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4577,8 +4571,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4594,8 +4588,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4608,10 +4602,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4658,72 +4652,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4798,60 +4792,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4860,10 +4854,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4878,10 +4872,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="28">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4897,10 +4891,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="28">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4916,10 +4910,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="28">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4935,8 +4929,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4952,8 +4946,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4969,8 +4963,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4983,10 +4977,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="55"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5033,72 +5027,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="37"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5126,16 +5120,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5148,24 +5150,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5190,64 +5184,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5258,8 +5252,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5270,8 +5264,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5282,8 +5276,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5294,8 +5288,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5306,8 +5300,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5318,8 +5312,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5329,8 +5323,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5374,52 +5368,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5429,9 +5423,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5518,60 +5512,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5582,10 +5576,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="54"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5600,10 +5594,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="28">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5619,10 +5613,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="28">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5638,10 +5632,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="28">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5657,8 +5651,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5674,8 +5668,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5691,10 +5685,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="53">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="53"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5707,10 +5701,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="63" t="s">
+      <c r="D39" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="64"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5757,58 +5751,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="32" t="s">
+      <c r="H43" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="37"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="33" t="s">
+      <c r="H46" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5818,12 +5812,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5836,32 +5856,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5887,177 +5881,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="65">
+      <c r="A5" s="67">
         <v>1</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="67">
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="66">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="66"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="65">
+      <c r="A7" s="67">
         <v>2</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67">
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="66">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="66"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="65">
+      <c r="A9" s="67">
         <v>3</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67">
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="66">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="67"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="66"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="65">
+      <c r="A11" s="67">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="67">
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="66">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="65"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="67"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="66"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="67">
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="66">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="67"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="66"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6068,10 +6062,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="54"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6086,8 +6080,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6103,10 +6097,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="28">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6122,8 +6116,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6139,10 +6133,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="28">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="28"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6158,8 +6152,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6175,10 +6169,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="53">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="53"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6191,10 +6185,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="64"/>
+      <c r="E32" s="58"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6241,58 +6235,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="32"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="32" t="s">
+      <c r="H36" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="37"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="33" t="s">
+      <c r="H39" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6302,12 +6296,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
@@ -6324,23 +6335,6 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
28.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 27.07.19</t>
+    <t>Date: 28.07.19</t>
   </si>
 </sst>
 </file>
@@ -447,47 +447,83 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -498,31 +534,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,15 +564,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -553,6 +577,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -573,37 +603,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2052,7 +2052,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2074,60 +2074,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2136,10 +2136,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2154,10 +2154,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2173,10 +2173,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2192,10 +2192,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2211,10 +2211,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2230,8 +2230,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2247,8 +2247,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2261,10 +2261,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2311,58 +2311,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2372,11 +2372,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2451,60 +2451,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2513,10 +2513,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="24"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2531,10 +2531,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2550,10 +2550,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2569,10 +2569,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2588,10 +2588,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2607,8 +2607,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2624,8 +2624,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2638,10 +2638,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="36"/>
+      <c r="E38" s="31"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2688,58 +2688,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="37"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="37" t="s">
+      <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="30" t="s">
+      <c r="H45" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2749,11 +2749,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="32" t="s">
+      <c r="H46" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2781,14 +2781,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2801,24 +2811,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2831,7 +2831,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="A1:K47"/>
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2894,32 +2894,32 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="74" t="s">
+      <c r="F5" s="46"/>
+      <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="4"/>
@@ -2933,13 +2933,13 @@
       <c r="D6" s="21">
         <v>1000</v>
       </c>
-      <c r="E6" s="47">
-        <v>60</v>
-      </c>
-      <c r="F6" s="47"/>
+      <c r="E6" s="42">
+        <v>30</v>
+      </c>
+      <c r="F6" s="42"/>
       <c r="G6" s="21">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2952,13 +2952,13 @@
       <c r="D7" s="21">
         <v>500</v>
       </c>
-      <c r="E7" s="47">
-        <v>340</v>
-      </c>
-      <c r="F7" s="47"/>
+      <c r="E7" s="42">
+        <v>194</v>
+      </c>
+      <c r="F7" s="42"/>
       <c r="G7" s="21">
         <f t="shared" si="0"/>
-        <v>170000</v>
+        <v>97000</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2971,13 +2971,13 @@
       <c r="D8" s="21">
         <v>100</v>
       </c>
-      <c r="E8" s="47">
-        <v>400</v>
-      </c>
-      <c r="F8" s="47"/>
+      <c r="E8" s="42">
+        <v>170</v>
+      </c>
+      <c r="F8" s="42"/>
       <c r="G8" s="21">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>17000</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2990,8 +2990,8 @@
       <c r="D9" s="21">
         <v>50</v>
       </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3007,8 +3007,8 @@
       <c r="D10" s="21">
         <v>20</v>
       </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3024,8 +3024,8 @@
       <c r="D11" s="21">
         <v>10</v>
       </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3038,14 +3038,14 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="75" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="76">
+      <c r="E12" s="46"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27">
         <f>SUM(G6:G11)</f>
-        <v>270000</v>
+        <v>144000</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3088,48 +3088,48 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
       <c r="H19" s="49" t="s">
         <v>12</v>
       </c>
@@ -3144,9 +3144,9 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4"/>
@@ -3261,32 +3261,32 @@
       <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="4" t="s">
@@ -3294,14 +3294,14 @@
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="D32" s="69" t="s">
+      <c r="D32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="70"/>
-      <c r="G32" s="69" t="s">
+      <c r="F32" s="57"/>
+      <c r="G32" s="24" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="4"/>
@@ -3315,13 +3315,13 @@
       <c r="D33" s="23">
         <v>1000</v>
       </c>
-      <c r="E33" s="47">
-        <v>60</v>
-      </c>
-      <c r="F33" s="47"/>
+      <c r="E33" s="42">
+        <v>30</v>
+      </c>
+      <c r="F33" s="42"/>
       <c r="G33" s="23">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -3334,13 +3334,13 @@
       <c r="D34" s="23">
         <v>500</v>
       </c>
-      <c r="E34" s="47">
-        <v>340</v>
-      </c>
-      <c r="F34" s="47"/>
+      <c r="E34" s="42">
+        <v>194</v>
+      </c>
+      <c r="F34" s="42"/>
       <c r="G34" s="23">
         <f t="shared" si="1"/>
-        <v>170000</v>
+        <v>97000</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -3353,13 +3353,13 @@
       <c r="D35" s="23">
         <v>100</v>
       </c>
-      <c r="E35" s="47">
-        <v>400</v>
-      </c>
-      <c r="F35" s="47"/>
+      <c r="E35" s="42">
+        <v>170</v>
+      </c>
+      <c r="F35" s="42"/>
       <c r="G35" s="23">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>17000</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3372,8 +3372,8 @@
       <c r="D36" s="23">
         <v>50</v>
       </c>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
       <c r="G36" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3389,8 +3389,8 @@
       <c r="D37" s="23">
         <v>20</v>
       </c>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="23">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3406,8 +3406,8 @@
       <c r="D38" s="23">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3420,14 +3420,14 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="71" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="72"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="73">
+      <c r="E39" s="55"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="25">
         <f>SUM(G33:G38)</f>
-        <v>270000</v>
+        <v>144000</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -3470,48 +3470,48 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="40"/>
-      <c r="H43" s="40" t="s">
+      <c r="B43" s="52"/>
+      <c r="H43" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
-      <c r="H46" s="42" t="s">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="H46" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3521,9 +3521,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3551,28 +3551,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3589,6 +3567,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3619,63 +3619,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3685,10 +3685,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3703,10 +3703,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3722,10 +3722,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3741,10 +3741,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3760,10 +3760,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3779,10 +3779,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,8 +3798,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3812,10 +3812,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3862,76 +3862,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="50"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4006,60 +4006,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4068,10 +4068,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="54" t="s">
+      <c r="E31" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="54"/>
+      <c r="F31" s="58"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4086,10 +4086,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="53">
+      <c r="E32" s="62">
         <v>68</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4105,10 +4105,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="53">
+      <c r="E33" s="62">
         <v>135</v>
       </c>
-      <c r="F33" s="53"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4124,10 +4124,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="53">
+      <c r="E34" s="62">
         <v>53</v>
       </c>
-      <c r="F34" s="53"/>
+      <c r="F34" s="62"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4143,10 +4143,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="53">
+      <c r="E35" s="62">
         <v>2</v>
       </c>
-      <c r="F35" s="53"/>
+      <c r="F35" s="62"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4162,10 +4162,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="53">
+      <c r="E36" s="62">
         <v>5</v>
       </c>
-      <c r="F36" s="53"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,8 +4181,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4195,10 +4195,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="52"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4245,76 +4245,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="37"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="37" t="s">
+      <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="30"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="30" t="s">
+      <c r="H45" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="51"/>
+      <c r="B46" s="60"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="32" t="s">
+      <c r="H46" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4342,30 +4342,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4382,6 +4358,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4413,63 +4413,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4479,10 +4479,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4497,10 +4497,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4516,10 +4516,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4535,10 +4535,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4554,8 +4554,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4571,8 +4571,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4588,8 +4588,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4602,10 +4602,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4652,72 +4652,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4792,60 +4792,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="25"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4854,10 +4854,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="24"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4872,10 +4872,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4891,10 +4891,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4910,10 +4910,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4929,8 +4929,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4946,8 +4946,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4963,8 +4963,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4977,10 +4977,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="55" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="55"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5027,72 +5027,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="37"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="37" t="s">
+      <c r="H42" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
+      <c r="A43" s="33"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="30" t="s">
+      <c r="H45" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="51"/>
-      <c r="B46" s="51"/>
+      <c r="A46" s="60"/>
+      <c r="B46" s="60"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="32" t="s">
+      <c r="H46" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5120,6 +5120,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5132,34 +5160,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5184,64 +5184,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5252,8 +5252,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5264,8 +5264,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5276,8 +5276,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5288,8 +5288,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5300,8 +5300,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5312,8 +5312,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5323,8 +5323,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5368,52 +5368,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5423,9 +5423,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5512,60 +5512,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5576,10 +5576,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="54" t="s">
+      <c r="E32" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="54"/>
+      <c r="F32" s="58"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5594,10 +5594,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="28"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5613,10 +5613,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="28">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="28"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5632,10 +5632,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="28"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5651,8 +5651,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5668,8 +5668,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5685,10 +5685,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
+      <c r="E38" s="62">
         <v>100</v>
       </c>
-      <c r="F38" s="53"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5701,10 +5701,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="57" t="s">
+      <c r="D39" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="58"/>
+      <c r="E39" s="66"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5751,58 +5751,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="37"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="37" t="s">
+      <c r="H43" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5812,20 +5812,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5838,24 +5848,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5881,177 +5881,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="67">
+      <c r="A5" s="68">
         <v>1</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="66">
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="67">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="67"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="66"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="67"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="67">
+      <c r="A7" s="68">
         <v>2</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="66">
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="67">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="67"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="66"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="67">
+      <c r="A9" s="68">
         <v>3</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="66">
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="67">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="67"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="66"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="67">
+      <c r="A11" s="68">
         <v>4</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="66">
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="67">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="67"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="66"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="66">
+      <c r="B13" s="76"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="67">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="68"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="66"/>
+      <c r="A14" s="76"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="67"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6062,10 +6062,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="54"/>
+      <c r="F25" s="58"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6080,8 +6080,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6097,10 +6097,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="28"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6116,8 +6116,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6133,10 +6133,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="28"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6152,8 +6152,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6169,10 +6169,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="53">
+      <c r="E31" s="62">
         <v>2</v>
       </c>
-      <c r="F31" s="53"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6185,10 +6185,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="57" t="s">
+      <c r="D32" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="58"/>
+      <c r="E32" s="66"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6235,58 +6235,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="37"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="37" t="s">
+      <c r="H36" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="30" t="s">
+      <c r="H39" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6296,12 +6296,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="33"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
@@ -6318,23 +6335,6 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
29.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 28.07.19</t>
+    <t>Date: 29.07.19</t>
   </si>
 </sst>
 </file>
@@ -459,12 +459,39 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -474,45 +501,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,90 +547,63 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2052,7 +2052,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2074,60 +2074,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2136,10 +2136,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2154,10 +2154,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2173,10 +2173,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2192,10 +2192,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2211,10 +2211,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2230,8 +2230,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2247,8 +2247,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2261,10 +2261,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2311,58 +2311,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2372,11 +2372,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2451,60 +2451,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2513,10 +2513,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2531,10 +2531,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="32">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2550,10 +2550,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2569,10 +2569,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="32">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2588,10 +2588,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="32">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2607,8 +2607,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2624,8 +2624,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2638,10 +2638,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2688,58 +2688,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2749,11 +2749,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2781,6 +2781,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2793,32 +2819,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2830,7 +2830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2849,63 +2849,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2915,10 +2915,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -2933,13 +2933,13 @@
       <c r="D6" s="21">
         <v>1000</v>
       </c>
-      <c r="E6" s="42">
-        <v>30</v>
-      </c>
-      <c r="F6" s="42"/>
+      <c r="E6" s="54">
+        <v>53</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="21">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>30000</v>
+        <v>53000</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2952,13 +2952,13 @@
       <c r="D7" s="21">
         <v>500</v>
       </c>
-      <c r="E7" s="42">
-        <v>194</v>
-      </c>
-      <c r="F7" s="42"/>
+      <c r="E7" s="54">
+        <v>111</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="21">
         <f t="shared" si="0"/>
-        <v>97000</v>
+        <v>55500</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2971,13 +2971,13 @@
       <c r="D8" s="21">
         <v>100</v>
       </c>
-      <c r="E8" s="42">
-        <v>170</v>
-      </c>
-      <c r="F8" s="42"/>
+      <c r="E8" s="54">
+        <v>282</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="21">
         <f t="shared" si="0"/>
-        <v>17000</v>
+        <v>28200</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2990,11 +2990,13 @@
       <c r="D9" s="21">
         <v>50</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+      <c r="E9" s="54">
+        <v>166</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8300</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -3007,11 +3009,13 @@
       <c r="D10" s="21">
         <v>20</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="54">
+        <v>400</v>
+      </c>
+      <c r="F10" s="54"/>
       <c r="G10" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3024,11 +3028,13 @@
       <c r="D11" s="21">
         <v>10</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+      <c r="E11" s="54">
+        <v>300</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -3038,14 +3044,14 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="26"/>
       <c r="G12" s="27">
         <f>SUM(G6:G11)</f>
-        <v>144000</v>
+        <v>156000</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3088,53 +3094,53 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
-      <c r="H19" s="49" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="H19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4"/>
@@ -3144,9 +3150,9 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4"/>
@@ -3233,60 +3239,60 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="4" t="s">
@@ -3297,10 +3303,10 @@
       <c r="D32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="24" t="s">
         <v>5</v>
       </c>
@@ -3315,13 +3321,13 @@
       <c r="D33" s="23">
         <v>1000</v>
       </c>
-      <c r="E33" s="42">
-        <v>30</v>
-      </c>
-      <c r="F33" s="42"/>
+      <c r="E33" s="54">
+        <v>53</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="23">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>30000</v>
+        <v>53000</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -3334,13 +3340,13 @@
       <c r="D34" s="23">
         <v>500</v>
       </c>
-      <c r="E34" s="42">
-        <v>194</v>
-      </c>
-      <c r="F34" s="42"/>
+      <c r="E34" s="54">
+        <v>111</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="23">
         <f t="shared" si="1"/>
-        <v>97000</v>
+        <v>55500</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -3353,13 +3359,13 @@
       <c r="D35" s="23">
         <v>100</v>
       </c>
-      <c r="E35" s="42">
-        <v>170</v>
-      </c>
-      <c r="F35" s="42"/>
+      <c r="E35" s="54">
+        <v>282</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="23">
         <f t="shared" si="1"/>
-        <v>17000</v>
+        <v>28200</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3372,11 +3378,13 @@
       <c r="D36" s="23">
         <v>50</v>
       </c>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="E36" s="54">
+        <v>166</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8300</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -3389,11 +3397,13 @@
       <c r="D37" s="23">
         <v>20</v>
       </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
+      <c r="E37" s="54">
+        <v>400</v>
+      </c>
+      <c r="F37" s="54"/>
       <c r="G37" s="23">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -3406,11 +3416,13 @@
       <c r="D38" s="23">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
+      <c r="E38" s="54">
+        <v>300</v>
+      </c>
+      <c r="F38" s="54"/>
       <c r="G38" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -3420,14 +3432,14 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="24"/>
       <c r="G39" s="25">
         <f>SUM(G33:G38)</f>
-        <v>144000</v>
+        <v>156000</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -3470,48 +3482,48 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="52" t="s">
+      <c r="A43" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="52"/>
-      <c r="H43" s="52" t="s">
+      <c r="B43" s="44"/>
+      <c r="H43" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
-      <c r="H46" s="53" t="s">
+      <c r="A46" s="45"/>
+      <c r="B46" s="45"/>
+      <c r="H46" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3521,9 +3533,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3551,6 +3563,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3567,28 +3601,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3619,63 +3631,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3685,10 +3697,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3703,10 +3715,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3722,10 +3734,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3741,10 +3753,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3760,10 +3772,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3779,10 +3791,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,8 +3810,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3812,10 +3824,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3862,76 +3874,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="59"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4006,60 +4018,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4068,10 +4080,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="58" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="58"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4086,10 +4098,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="62">
+      <c r="E32" s="61">
         <v>68</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4105,10 +4117,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="61">
         <v>135</v>
       </c>
-      <c r="F33" s="62"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4124,10 +4136,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="61">
         <v>53</v>
       </c>
-      <c r="F34" s="62"/>
+      <c r="F34" s="61"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4143,10 +4155,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="61">
         <v>2</v>
       </c>
-      <c r="F35" s="62"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4162,10 +4174,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="62">
+      <c r="E36" s="61">
         <v>5</v>
       </c>
-      <c r="F36" s="62"/>
+      <c r="F36" s="61"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,8 +4193,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4195,10 +4207,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="60"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4245,76 +4257,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="60"/>
+      <c r="B46" s="59"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4342,6 +4354,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4358,30 +4394,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4413,63 +4425,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4479,10 +4491,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4497,10 +4509,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4516,10 +4528,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4535,10 +4547,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4554,8 +4566,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4571,8 +4583,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4588,8 +4600,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4602,10 +4614,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4652,72 +4664,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4792,60 +4804,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4854,10 +4866,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4872,10 +4884,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="32">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4891,10 +4903,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4910,10 +4922,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="32">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4929,8 +4941,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4946,8 +4958,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4963,8 +4975,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4977,10 +4989,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="63"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5027,72 +5039,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="60"/>
-      <c r="B46" s="60"/>
+      <c r="A46" s="59"/>
+      <c r="B46" s="59"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5120,16 +5132,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5142,24 +5162,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5184,64 +5196,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5252,8 +5264,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5264,8 +5276,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5276,8 +5288,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5288,8 +5300,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5300,8 +5312,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5312,8 +5324,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5323,8 +5335,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5368,52 +5380,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5423,9 +5435,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5512,60 +5524,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5576,10 +5588,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="58"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5594,10 +5606,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5613,10 +5625,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="32">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5632,10 +5644,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="32">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5651,8 +5663,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5668,8 +5680,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5685,10 +5697,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="62">
+      <c r="E38" s="61">
         <v>100</v>
       </c>
-      <c r="F38" s="62"/>
+      <c r="F38" s="61"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5751,58 +5763,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="32" t="s">
+      <c r="H43" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="33" t="s">
+      <c r="H46" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5812,12 +5824,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5830,32 +5868,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5881,177 +5893,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="68">
+      <c r="A5" s="76">
         <v>1</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="67">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="75">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="68"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="75"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="68">
+      <c r="A7" s="76">
         <v>2</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="67">
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="75">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="68"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="67"/>
+      <c r="A8" s="76"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="75"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="68">
+      <c r="A9" s="76">
         <v>3</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="67">
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="75">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="68"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="67"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="75"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="68">
+      <c r="A11" s="76">
         <v>4</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="67">
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="75">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="68"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="67"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="75"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="67">
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="75">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="76"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="67"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="75"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6062,10 +6074,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="58"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6080,8 +6092,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6097,10 +6109,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="32">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6116,8 +6128,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6133,10 +6145,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="32">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6152,8 +6164,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6169,10 +6181,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="62">
+      <c r="E31" s="61">
         <v>2</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="61"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6235,58 +6247,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="32"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="32" t="s">
+      <c r="H36" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="33" t="s">
+      <c r="H39" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6296,29 +6308,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B9:F10"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H40:J40"/>
@@ -6335,6 +6330,23 @@
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B9:F10"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
31.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/July/Others/Cash.xlsx
+++ b/July/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 30.07.19</t>
+    <t>Date: 31.07.19</t>
   </si>
 </sst>
 </file>
@@ -459,12 +459,39 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -474,45 +501,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,56 +547,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -577,31 +577,31 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2052,7 +2052,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2074,60 +2074,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2136,10 +2136,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2154,10 +2154,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2173,10 +2173,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2192,10 +2192,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2211,10 +2211,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2230,8 +2230,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2247,8 +2247,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2261,10 +2261,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2311,58 +2311,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2372,11 +2372,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2451,60 +2451,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2513,10 +2513,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2531,10 +2531,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="32">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2550,10 +2550,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2569,10 +2569,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="32">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2588,10 +2588,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="32">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2607,8 +2607,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2624,8 +2624,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2638,10 +2638,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="40"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2688,58 +2688,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2749,11 +2749,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2781,6 +2781,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2793,32 +2819,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2830,7 +2830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2849,63 +2849,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2915,10 +2915,10 @@
       <c r="D5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
@@ -2933,13 +2933,13 @@
       <c r="D6" s="21">
         <v>1000</v>
       </c>
-      <c r="E6" s="42">
-        <v>94</v>
-      </c>
-      <c r="F6" s="42"/>
+      <c r="E6" s="54">
+        <v>100</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="21">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>94000</v>
+        <v>100000</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2952,13 +2952,13 @@
       <c r="D7" s="21">
         <v>500</v>
       </c>
-      <c r="E7" s="42">
-        <v>150</v>
-      </c>
-      <c r="F7" s="42"/>
+      <c r="E7" s="54">
+        <v>302</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="21">
         <f t="shared" si="0"/>
-        <v>75000</v>
+        <v>151000</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2971,13 +2971,13 @@
       <c r="D8" s="21">
         <v>100</v>
       </c>
-      <c r="E8" s="42">
-        <v>300</v>
-      </c>
-      <c r="F8" s="42"/>
+      <c r="E8" s="54">
+        <v>521</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="21">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>52100</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2990,13 +2990,13 @@
       <c r="D9" s="21">
         <v>50</v>
       </c>
-      <c r="E9" s="42">
-        <v>120</v>
-      </c>
-      <c r="F9" s="42"/>
+      <c r="E9" s="54">
+        <v>186</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="21">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>9300</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -3009,13 +3009,13 @@
       <c r="D10" s="21">
         <v>20</v>
       </c>
-      <c r="E10" s="42">
-        <v>0</v>
-      </c>
-      <c r="F10" s="42"/>
+      <c r="E10" s="54">
+        <v>80</v>
+      </c>
+      <c r="F10" s="54"/>
       <c r="G10" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3028,13 +3028,13 @@
       <c r="D11" s="21">
         <v>10</v>
       </c>
-      <c r="E11" s="42">
-        <v>200</v>
-      </c>
-      <c r="F11" s="42"/>
+      <c r="E11" s="54">
+        <v>100</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="21">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -3044,14 +3044,14 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="26"/>
       <c r="G12" s="27">
         <f>SUM(G6:G11)</f>
-        <v>207000</v>
+        <v>315000</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3094,53 +3094,53 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
-      <c r="H19" s="49" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="45"/>
+      <c r="H19" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4"/>
@@ -3150,9 +3150,9 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4"/>
@@ -3239,60 +3239,60 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="4" t="s">
@@ -3303,10 +3303,10 @@
       <c r="D32" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="24" t="s">
         <v>5</v>
       </c>
@@ -3321,13 +3321,13 @@
       <c r="D33" s="23">
         <v>1000</v>
       </c>
-      <c r="E33" s="42">
-        <v>94</v>
-      </c>
-      <c r="F33" s="42"/>
+      <c r="E33" s="54">
+        <v>100</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="23">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>94000</v>
+        <v>100000</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -3340,13 +3340,13 @@
       <c r="D34" s="23">
         <v>500</v>
       </c>
-      <c r="E34" s="42">
-        <v>150</v>
-      </c>
-      <c r="F34" s="42"/>
+      <c r="E34" s="54">
+        <v>302</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="23">
         <f t="shared" si="1"/>
-        <v>75000</v>
+        <v>151000</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -3359,13 +3359,13 @@
       <c r="D35" s="23">
         <v>100</v>
       </c>
-      <c r="E35" s="42">
-        <v>300</v>
-      </c>
-      <c r="F35" s="42"/>
+      <c r="E35" s="54">
+        <v>521</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="23">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>52100</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -3378,13 +3378,13 @@
       <c r="D36" s="23">
         <v>50</v>
       </c>
-      <c r="E36" s="42">
-        <v>120</v>
-      </c>
-      <c r="F36" s="42"/>
+      <c r="E36" s="54">
+        <v>186</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="23">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>9300</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -3397,13 +3397,13 @@
       <c r="D37" s="23">
         <v>20</v>
       </c>
-      <c r="E37" s="42">
-        <v>0</v>
-      </c>
-      <c r="F37" s="42"/>
+      <c r="E37" s="54">
+        <v>80</v>
+      </c>
+      <c r="F37" s="54"/>
       <c r="G37" s="23">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -3416,13 +3416,13 @@
       <c r="D38" s="23">
         <v>10</v>
       </c>
-      <c r="E38" s="42">
-        <v>200</v>
-      </c>
-      <c r="F38" s="42"/>
+      <c r="E38" s="54">
+        <v>100</v>
+      </c>
+      <c r="F38" s="54"/>
       <c r="G38" s="23">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
@@ -3432,14 +3432,14 @@
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="24"/>
       <c r="G39" s="25">
         <f>SUM(G33:G38)</f>
-        <v>207000</v>
+        <v>315000</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -3482,48 +3482,48 @@
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="52" t="s">
+      <c r="A43" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="52"/>
-      <c r="H43" s="52" t="s">
+      <c r="B43" s="44"/>
+      <c r="H43" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
-      <c r="H46" s="53" t="s">
+      <c r="A46" s="45"/>
+      <c r="B46" s="45"/>
+      <c r="H46" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3533,9 +3533,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3563,6 +3563,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3579,28 +3601,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3631,63 +3631,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3697,10 +3697,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3715,10 +3715,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3734,10 +3734,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3753,10 +3753,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3772,10 +3772,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3791,10 +3791,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3810,8 +3810,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3824,10 +3824,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3874,76 +3874,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="59"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4018,60 +4018,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4080,10 +4080,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="58" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="58"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4098,10 +4098,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="62">
+      <c r="E32" s="61">
         <v>68</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="61"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4117,10 +4117,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="61">
         <v>135</v>
       </c>
-      <c r="F33" s="62"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4136,10 +4136,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="61">
         <v>53</v>
       </c>
-      <c r="F34" s="62"/>
+      <c r="F34" s="61"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4155,10 +4155,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="61">
         <v>2</v>
       </c>
-      <c r="F35" s="62"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4174,10 +4174,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="62">
+      <c r="E36" s="61">
         <v>5</v>
       </c>
-      <c r="F36" s="62"/>
+      <c r="F36" s="61"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4193,8 +4193,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4207,10 +4207,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="60"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4257,76 +4257,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="60"/>
+      <c r="B46" s="59"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4354,6 +4354,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4370,30 +4394,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4425,63 +4425,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4491,10 +4491,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4509,10 +4509,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4528,10 +4528,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4547,10 +4547,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4566,8 +4566,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4583,8 +4583,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4600,8 +4600,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4614,10 +4614,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4664,72 +4664,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4804,60 +4804,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4866,10 +4866,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4884,10 +4884,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="32">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4903,10 +4903,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4922,10 +4922,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="32">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4941,8 +4941,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4958,8 +4958,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4975,8 +4975,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4989,10 +4989,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="63"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5039,72 +5039,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="32"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="33"/>
-      <c r="B43" s="33"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="60"/>
-      <c r="B46" s="60"/>
+      <c r="A46" s="59"/>
+      <c r="B46" s="59"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="28" t="s">
+      <c r="H46" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5132,16 +5132,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5154,24 +5162,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5196,64 +5196,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5264,8 +5264,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5276,8 +5276,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5288,8 +5288,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5300,8 +5300,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5312,8 +5312,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5324,8 +5324,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5335,8 +5335,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5380,52 +5380,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5435,9 +5435,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5524,60 +5524,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5588,10 +5588,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="58"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5606,10 +5606,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="32">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5625,10 +5625,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="32">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5644,10 +5644,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="32">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5663,8 +5663,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5680,8 +5680,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5697,10 +5697,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="62">
+      <c r="E38" s="61">
         <v>100</v>
       </c>
-      <c r="F38" s="62"/>
+      <c r="F38" s="61"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5763,58 +5763,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="32"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="32" t="s">
+      <c r="H43" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="33"/>
-      <c r="B44" s="33"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="33"/>
-      <c r="B45" s="33"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="33"/>
-      <c r="J45" s="33"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="33"/>
-      <c r="B46" s="33"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="33" t="s">
+      <c r="H46" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5824,12 +5824,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5842,32 +5868,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5893,128 +5893,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="68">
+      <c r="A5" s="75">
         <v>1</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="67">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="74">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="68"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="67"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="74"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="68">
+      <c r="A7" s="75">
         <v>2</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="67">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="74">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="68"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="67"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="74"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="68">
+      <c r="A9" s="75">
         <v>3</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="67">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="74">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="68"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="67"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="74"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="68">
+      <c r="A11" s="75">
         <v>4</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="67">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="74">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="68"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="67"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="74"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="76" t="s">
@@ -6025,7 +6025,7 @@
       <c r="D13" s="76"/>
       <c r="E13" s="76"/>
       <c r="F13" s="76"/>
-      <c r="G13" s="67">
+      <c r="G13" s="74">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
@@ -6037,33 +6037,33 @@
       <c r="D14" s="76"/>
       <c r="E14" s="76"/>
       <c r="F14" s="76"/>
-      <c r="G14" s="67"/>
+      <c r="G14" s="74"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6074,10 +6074,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="58"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6092,8 +6092,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6109,10 +6109,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="32">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6128,8 +6128,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6145,10 +6145,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="32">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6164,8 +6164,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6181,10 +6181,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="62">
+      <c r="E31" s="61">
         <v>2</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="61"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6247,58 +6247,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="32"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="32" t="s">
+      <c r="H36" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="33"/>
-      <c r="B37" s="33"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="33"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="33"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="33" t="s">
+      <c r="H39" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6308,12 +6308,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="28"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
@@ -6330,23 +6347,6 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="E26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>